<commit_message>
work on BDO and lipidcane
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Element</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Natural gas consumption [MMcf/yr]</t>
-  </si>
-  <si>
-    <t>Productivity [MMGGE/yr]</t>
   </si>
   <si>
     <t>TCI [10^6*USD]</t>
@@ -452,13 +449,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,9 +469,8 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:10">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -502,301 +498,268 @@
       <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>0.03827795694892373</v>
+        <v>0.02622262226222622</v>
       </c>
       <c r="E4">
-        <v>-0.06076201905047627</v>
+        <v>0.05513351335133513</v>
       </c>
       <c r="F4">
-        <v>-0.0615705392634816</v>
+        <v>0.07425142514251425</v>
       </c>
       <c r="H4">
-        <v>-0.06061201530038251</v>
+        <v>0.06303030303030302</v>
       </c>
       <c r="I4">
-        <v>-0.08230255756393912</v>
+        <v>0.06549054905490548</v>
       </c>
       <c r="J4">
-        <v>-0.06124653116327909</v>
-      </c>
-      <c r="K4">
-        <v>-0.1786313904618974</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>-0.06365836848766269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>0.02411910297757444</v>
+        <v>0.1291689168916892</v>
       </c>
       <c r="E5">
-        <v>0.147275181879547</v>
+        <v>0.0003000300030002999</v>
       </c>
       <c r="F5">
-        <v>0.1328433210830271</v>
+        <v>0.007116711671167116</v>
       </c>
       <c r="H5">
-        <v>0.1412060301507538</v>
+        <v>-0.06853885388538854</v>
       </c>
       <c r="I5">
-        <v>0.08813020325508138</v>
+        <v>0.007644764476447644</v>
       </c>
       <c r="J5">
-        <v>0.1361659041476037</v>
-      </c>
-      <c r="K5">
-        <v>0.0214747381950692</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>0.09616298104940993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>-0.003130578264456612</v>
+        <v>-0.04182418241824182</v>
       </c>
       <c r="E6">
-        <v>-0.05567389184729619</v>
+        <v>-0.07277527752775277</v>
       </c>
       <c r="F6">
-        <v>-0.06841071026775671</v>
+        <v>-0.08244824482448244</v>
       </c>
       <c r="H6">
-        <v>-0.05884647116177905</v>
+        <v>-0.01870987098709871</v>
       </c>
       <c r="I6">
-        <v>-0.06852771319282984</v>
+        <v>-0.0738073807380738</v>
       </c>
       <c r="J6">
-        <v>-0.06355658891472288</v>
-      </c>
-      <c r="K6">
-        <v>-0.004521155414916079</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>0.006273978597529711</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>0.03228322832283228</v>
+      </c>
+      <c r="E7">
+        <v>0.7706330633063305</v>
+      </c>
+      <c r="F7">
+        <v>0.7708610861086107</v>
+      </c>
+      <c r="H7">
+        <v>0.9997839783978397</v>
+      </c>
+      <c r="I7">
+        <v>0.7682568256825681</v>
+      </c>
+      <c r="J7">
+        <v>-0.1074561425249634</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7">
-        <v>0.083625590639766</v>
-      </c>
-      <c r="E7">
-        <v>0.7677551938798471</v>
-      </c>
-      <c r="F7">
-        <v>0.784926123153079</v>
-      </c>
-      <c r="H7">
-        <v>0.7736998424960625</v>
-      </c>
-      <c r="I7">
-        <v>0.9997479936998426</v>
-      </c>
-      <c r="J7">
-        <v>0.7776224405610143</v>
-      </c>
-      <c r="K7">
-        <v>0.2443216485674067</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
+      <c r="C8">
+        <v>0.9654965496549653</v>
+      </c>
+      <c r="E8">
+        <v>0.05034503450345034</v>
+      </c>
+      <c r="F8">
+        <v>0.04788478847884788</v>
+      </c>
+      <c r="H8">
+        <v>0.01663366336633663</v>
+      </c>
+      <c r="I8">
+        <v>0.0403000300030003</v>
+      </c>
+      <c r="J8">
+        <v>0.1220453941919464</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>0.134029402940294</v>
+      </c>
+      <c r="E9">
+        <v>0.1125112511251125</v>
+      </c>
+      <c r="F9">
+        <v>0.1123072307230723</v>
+      </c>
+      <c r="H9">
+        <v>0.121980198019802</v>
+      </c>
+      <c r="I9">
+        <v>0.1078307830783078</v>
+      </c>
+      <c r="J9">
+        <v>0.1595031477517434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8">
-        <v>0.9619410485262132</v>
-      </c>
-      <c r="E8">
-        <v>0.03296332408310208</v>
-      </c>
-      <c r="F8">
-        <v>0.02788269706742669</v>
-      </c>
-      <c r="H8">
-        <v>0.03044326108152704</v>
-      </c>
-      <c r="I8">
-        <v>0.04204455111377785</v>
-      </c>
-      <c r="J8">
-        <v>0.02759318982974574</v>
-      </c>
-      <c r="K8">
-        <v>-0.0003735128395202732</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9">
-        <v>-0.01385134628365709</v>
-      </c>
-      <c r="E9">
-        <v>-0.02006750168754219</v>
-      </c>
-      <c r="F9">
-        <v>-0.02130203255081378</v>
-      </c>
-      <c r="H9">
-        <v>-0.01914647866196655</v>
-      </c>
-      <c r="I9">
-        <v>0.02135753393834846</v>
-      </c>
-      <c r="J9">
-        <v>-0.01898597464936624</v>
-      </c>
-      <c r="K9">
-        <v>0.02700017813230987</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="1" t="s">
+      <c r="C10">
+        <v>0.00522052205220522</v>
+      </c>
+      <c r="E10">
+        <v>0.1051905190519052</v>
+      </c>
+      <c r="F10">
+        <v>0.1362976297629763</v>
+      </c>
+      <c r="H10">
+        <v>-0.02341434143414341</v>
+      </c>
+      <c r="I10">
+        <v>0.123048304830483</v>
+      </c>
+      <c r="J10">
+        <v>-0.02253829249294405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10">
-        <v>0.113422335558389</v>
-      </c>
-      <c r="E10">
-        <v>-0.003007575189379735</v>
-      </c>
-      <c r="F10">
-        <v>-0.01413485337133429</v>
-      </c>
-      <c r="H10">
-        <v>-0.00570014250356259</v>
-      </c>
-      <c r="I10">
-        <v>-0.03300832520813021</v>
-      </c>
-      <c r="J10">
-        <v>-0.0102377559438986</v>
-      </c>
-      <c r="K10">
-        <v>0.01896440190214881</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C11">
-        <v>0.04565964149103728</v>
+        <v>0.1054065406540654</v>
       </c>
       <c r="E11">
-        <v>0.103241581039526</v>
+        <v>-0.1616921692169217</v>
       </c>
       <c r="F11">
-        <v>0.09439585989649743</v>
+        <v>-0.1412901290129013</v>
       </c>
       <c r="H11">
-        <v>0.102137553438836</v>
+        <v>-0.1034623462346234</v>
       </c>
       <c r="I11">
-        <v>0.126651166279157</v>
+        <v>-0.1527512751275127</v>
       </c>
       <c r="J11">
-        <v>0.09863796594914874</v>
-      </c>
-      <c r="K11">
-        <v>0.03674076296534157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>-0.2168575186055245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>0.0834455861396535</v>
+        <v>0.1404740474047405</v>
       </c>
       <c r="E12">
-        <v>0.5355733893347334</v>
+        <v>0.4869126912691268</v>
       </c>
       <c r="F12">
-        <v>0.5154233855846397</v>
+        <v>0.4854965496549655</v>
       </c>
       <c r="H12">
-        <v>0.5315637890947275</v>
+        <v>-0.1544554455445544</v>
       </c>
       <c r="I12">
-        <v>-0.09208730218255458</v>
+        <v>0.4959975997599759</v>
       </c>
       <c r="J12">
-        <v>0.5283537088427211</v>
-      </c>
-      <c r="K12">
-        <v>-0.1738154749145888</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>0.03774593630877444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13">
-        <v>-0.2088097202430061</v>
+        <v>-0.2772277227722772</v>
       </c>
       <c r="E13">
-        <v>0.0003885097127428186</v>
+        <v>-0.008076807680768076</v>
       </c>
       <c r="F13">
-        <v>0.007132678316957926</v>
+        <v>0.005376537653765376</v>
       </c>
       <c r="H13">
-        <v>0.001819545488637216</v>
+        <v>0.00534053405340534</v>
       </c>
       <c r="I13">
-        <v>0.06145203630090753</v>
+        <v>-0.004776477647764776</v>
       </c>
       <c r="J13">
-        <v>0.004314107852696318</v>
-      </c>
-      <c r="K13">
-        <v>-0.02994177924997756</v>
+        <v>-0.1510858099586939</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="C1:J1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A11:A13"/>
   </mergeCells>

</xml_diff>

<commit_message>
add analyses to lipidcane2g
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Element</t>
   </si>
@@ -28,16 +28,16 @@
     <t>MFPP [USD/ton]</t>
   </si>
   <si>
-    <t>Biodiesel production [MMGal/yr]</t>
-  </si>
-  <si>
-    <t>Ethanol production [MMGal/yr]</t>
-  </si>
-  <si>
-    <t>Electricity production [MMWhr/yr]</t>
-  </si>
-  <si>
-    <t>Natural gas consumption [MMcf/yr]</t>
+    <t>Biodiesel production [Gal/ton]</t>
+  </si>
+  <si>
+    <t>Ethanol production [Gal/ton]</t>
+  </si>
+  <si>
+    <t>Electricity production [kWhr/ton]</t>
+  </si>
+  <si>
+    <t>Natural gas consumption [cf/ton]</t>
   </si>
   <si>
     <t>TCI [10^6*USD]</t>
@@ -47,6 +47,24 @@
   </si>
   <si>
     <t>Heat exchanger network error [%]</t>
+  </si>
+  <si>
+    <t>MFPP derivative [USD/ton]</t>
+  </si>
+  <si>
+    <t>Biodiesel production derivative [Gal/ton]</t>
+  </si>
+  <si>
+    <t>Ethanol production derivative [Gal/ton]</t>
+  </si>
+  <si>
+    <t>Electricity production derivative [kWhr/ton]</t>
+  </si>
+  <si>
+    <t>Natural gas consumption derivative [cf/ton]</t>
+  </si>
+  <si>
+    <t>TCI derivative [10^6*USD]</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -452,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +490,14 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -501,292 +525,310 @@
       <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C4">
-        <v>0.03318082952073802</v>
+        <v>0.0181917421917422</v>
       </c>
       <c r="E4">
-        <v>-0.05970599264981625</v>
+        <v>0.03897105897105898</v>
       </c>
       <c r="F4">
-        <v>-0.06618165454136354</v>
+        <v>-0.03058968658968659</v>
       </c>
       <c r="H4">
-        <v>-0.09006075151878798</v>
+        <v>-0.02466633666633667</v>
       </c>
       <c r="I4">
-        <v>-0.06155253881347034</v>
+        <v>-0.04342405942405943</v>
       </c>
       <c r="J4">
-        <v>0.08631424977000805</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>-0.001574413850395462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>-0.01987249681242031</v>
+        <v>0.003629079629079629</v>
       </c>
       <c r="E5">
-        <v>-0.008386709667741696</v>
+        <v>-0.02545645345645346</v>
       </c>
       <c r="F5">
-        <v>-0.02111902797569939</v>
+        <v>0.0234030234030234</v>
       </c>
       <c r="H5">
-        <v>-0.05913147828695718</v>
+        <v>0.05317775317775318</v>
       </c>
       <c r="I5">
-        <v>-0.01549088727218181</v>
+        <v>0.008772572772572774</v>
       </c>
       <c r="J5">
-        <v>-0.05579969442588657</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>-0.05550504720877538</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C6">
-        <v>0.09029475736893423</v>
+        <v>0.006859926859926861</v>
       </c>
       <c r="E6">
-        <v>0.01933098327458187</v>
+        <v>-0.03286205686205686</v>
       </c>
       <c r="F6">
-        <v>0.03489237230930774</v>
+        <v>0.0480894840894841</v>
       </c>
       <c r="H6">
-        <v>0.04719267981699543</v>
+        <v>0.03835268635268636</v>
       </c>
       <c r="I6">
-        <v>0.027875196879922</v>
+        <v>0.06633054633054633</v>
       </c>
       <c r="J6">
-        <v>-0.04843005085087737</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>-0.01569203843262542</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C7">
-        <v>0.09875196879921999</v>
+        <v>-0.06119233319233319</v>
       </c>
       <c r="E7">
-        <v>0.09669841746043652</v>
+        <v>0.05594164394164394</v>
       </c>
       <c r="F7">
-        <v>0.09395634890872273</v>
+        <v>-0.07022207822207822</v>
       </c>
       <c r="H7">
-        <v>0.1278331958298958</v>
+        <v>-0.04286944286944287</v>
       </c>
       <c r="I7">
-        <v>0.09733893347333686</v>
+        <v>-0.03785164985164986</v>
       </c>
       <c r="J7">
-        <v>-0.05599548809171285</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>0.05777622972827799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>0.03524002724002724</v>
+      </c>
+      <c r="E8">
+        <v>-0.3040925920925922</v>
+      </c>
+      <c r="F8">
+        <v>0.4903575223575223</v>
+      </c>
+      <c r="H8">
+        <v>0.9997759717759719</v>
+      </c>
+      <c r="I8">
+        <v>0.7924959484959485</v>
+      </c>
+      <c r="J8">
+        <v>-0.02086463484489577</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>0.964986796986797</v>
+      </c>
+      <c r="E9">
+        <v>0.01353000153000153</v>
+      </c>
+      <c r="F9">
+        <v>-0.01954833154833155</v>
+      </c>
+      <c r="H9">
+        <v>-0.0149016509016509</v>
+      </c>
+      <c r="I9">
+        <v>-0.01146227946227946</v>
+      </c>
+      <c r="J9">
+        <v>0.0221860640995974</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>-0.00473905673905674</v>
+      </c>
+      <c r="E10">
+        <v>0.02764022764022764</v>
+      </c>
+      <c r="F10">
+        <v>-0.01215200415200415</v>
+      </c>
+      <c r="H10">
+        <v>0.03131586731586732</v>
+      </c>
+      <c r="I10">
+        <v>0.04357605157605158</v>
+      </c>
+      <c r="J10">
+        <v>0.01826569431243045</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8">
-        <v>0.1037245931148279</v>
-      </c>
-      <c r="E8">
-        <v>0.7993909847746195</v>
-      </c>
-      <c r="F8">
-        <v>0.8142788569714243</v>
-      </c>
-      <c r="H8">
-        <v>0.9997359933998351</v>
-      </c>
-      <c r="I8">
-        <v>0.8048346208655217</v>
-      </c>
-      <c r="J8">
-        <v>-0.0798478076266266</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>-0.03709177309177309</v>
+      </c>
+      <c r="E11">
+        <v>-0.03686466086466087</v>
+      </c>
+      <c r="F11">
+        <v>0.0350929070929071</v>
+      </c>
+      <c r="H11">
+        <v>-0.04453786453786453</v>
+      </c>
+      <c r="I11">
+        <v>-0.05375321375321376</v>
+      </c>
+      <c r="J11">
+        <v>-0.01477993000562896</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9">
-        <v>0.9613335333383336</v>
-      </c>
-      <c r="E9">
-        <v>0.05336683417085427</v>
-      </c>
-      <c r="F9">
-        <v>0.06563564089102228</v>
-      </c>
-      <c r="H9">
-        <v>0.05123678091952299</v>
-      </c>
-      <c r="I9">
-        <v>0.05961899047476188</v>
-      </c>
-      <c r="J9">
-        <v>-0.2009585677006658</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10">
-        <v>0.005883147078676968</v>
-      </c>
-      <c r="E10">
-        <v>-0.03819245481137029</v>
-      </c>
-      <c r="F10">
-        <v>-0.05166129153228831</v>
-      </c>
-      <c r="H10">
-        <v>-0.1126513162829071</v>
-      </c>
-      <c r="I10">
-        <v>-0.04569414235355885</v>
-      </c>
-      <c r="J10">
-        <v>0.1143975128882943</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11">
-        <v>0.05945248631215781</v>
-      </c>
-      <c r="E11">
-        <v>0.07651241281032027</v>
-      </c>
-      <c r="F11">
-        <v>0.08558763969099227</v>
-      </c>
-      <c r="H11">
-        <v>0.091164779119478</v>
-      </c>
-      <c r="I11">
-        <v>0.08060751518787972</v>
-      </c>
-      <c r="J11">
-        <v>-0.03822627520885017</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C12">
-        <v>-0.02710267756693918</v>
+        <v>0.05256611256611257</v>
       </c>
       <c r="E12">
-        <v>-0.04477761944048602</v>
+        <v>-0.02651784251784252</v>
       </c>
       <c r="F12">
-        <v>-0.04905722643066077</v>
+        <v>0.03053051453051453</v>
       </c>
       <c r="H12">
-        <v>-0.03127578189454737</v>
+        <v>-0.01388286188286188</v>
       </c>
       <c r="I12">
-        <v>-0.04644566114152855</v>
+        <v>-0.02742773142773143</v>
       </c>
       <c r="J12">
-        <v>0.1292088160993063</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>-0.01184897533039653</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C13">
-        <v>0.1569369234230856</v>
+        <v>0.1031496791496792</v>
       </c>
       <c r="E13">
-        <v>0.6320048001200032</v>
+        <v>-0.005206961206961207</v>
       </c>
       <c r="F13">
-        <v>0.6135003375084378</v>
+        <v>0.003686595686595687</v>
       </c>
       <c r="H13">
-        <v>0.07281482037050928</v>
+        <v>-0.01794496194496194</v>
       </c>
       <c r="I13">
-        <v>0.6292117302932574</v>
+        <v>0.5802783162783164</v>
       </c>
       <c r="J13">
-        <v>-0.07161697198890256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>0.01807563320419748</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C14">
-        <v>-0.1893707342683567</v>
+        <v>-0.2292568092568093</v>
       </c>
       <c r="E14">
-        <v>0.01534988374709368</v>
+        <v>0.003102279102279102</v>
       </c>
       <c r="F14">
-        <v>0.02378309457736444</v>
+        <v>-0.0103978183978184</v>
       </c>
       <c r="H14">
-        <v>0.07134328358208956</v>
+        <v>-0.02445218445218445</v>
       </c>
       <c r="I14">
-        <v>0.01989949748743719</v>
+        <v>-0.02457429657429657</v>
       </c>
       <c r="J14">
-        <v>0.03251750204050529</v>
+        <v>0.04371730251872426</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C1:P1"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A12:A14"/>
   </mergeCells>

</xml_diff>

<commit_message>
more work on lipidcane analyses
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -560,22 +560,22 @@
         <v>23</v>
       </c>
       <c r="C4">
-        <v>0.0181917421917422</v>
+        <v>0.03895589558955895</v>
       </c>
       <c r="E4">
-        <v>0.03897105897105898</v>
+        <v>-0.06773477347734773</v>
       </c>
       <c r="F4">
-        <v>-0.03058968658968659</v>
+        <v>-0.006924692469246924</v>
       </c>
       <c r="H4">
-        <v>-0.02466633666633667</v>
+        <v>-0.06741074107410741</v>
       </c>
       <c r="I4">
-        <v>-0.04342405942405943</v>
+        <v>-0.01120912091209121</v>
       </c>
       <c r="J4">
-        <v>-0.001574413850395462</v>
+        <v>0.01022620393733763</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -584,22 +584,22 @@
         <v>24</v>
       </c>
       <c r="C5">
-        <v>0.003629079629079629</v>
+        <v>-0.1369216921692169</v>
       </c>
       <c r="E5">
-        <v>-0.02545645345645346</v>
+        <v>-0.01947794779477947</v>
       </c>
       <c r="F5">
-        <v>0.0234030234030234</v>
+        <v>-0.06955895589558955</v>
       </c>
       <c r="H5">
-        <v>0.05317775317775318</v>
+        <v>-0.06672667266726671</v>
       </c>
       <c r="I5">
-        <v>0.008772572772572774</v>
+        <v>-0.1615121512151215</v>
       </c>
       <c r="J5">
-        <v>-0.05550504720877538</v>
+        <v>-0.000492395022232346</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -608,22 +608,22 @@
         <v>25</v>
       </c>
       <c r="C6">
-        <v>0.006859926859926861</v>
+        <v>0.04655265526552655</v>
       </c>
       <c r="E6">
-        <v>-0.03286205686205686</v>
+        <v>0.1524872487248725</v>
       </c>
       <c r="F6">
-        <v>0.0480894840894841</v>
+        <v>-0.06835883588358835</v>
       </c>
       <c r="H6">
-        <v>0.03835268635268636</v>
+        <v>-0.0144974497449745</v>
       </c>
       <c r="I6">
-        <v>0.06633054633054633</v>
+        <v>-0.05526552655265525</v>
       </c>
       <c r="J6">
-        <v>-0.01569203843262542</v>
+        <v>-0.04121706625125394</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -632,22 +632,22 @@
         <v>26</v>
       </c>
       <c r="C7">
-        <v>-0.06119233319233319</v>
+        <v>-0.003708370837083708</v>
       </c>
       <c r="E7">
-        <v>0.05594164394164394</v>
+        <v>0.06589858985898589</v>
       </c>
       <c r="F7">
-        <v>-0.07022207822207822</v>
+        <v>-0.0287068706870687</v>
       </c>
       <c r="H7">
-        <v>-0.04286944286944287</v>
+        <v>0.006540654065406539</v>
       </c>
       <c r="I7">
-        <v>-0.03785164985164986</v>
+        <v>0.004116411641164116</v>
       </c>
       <c r="J7">
-        <v>0.05777622972827799</v>
+        <v>-0.02175545323838768</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -656,22 +656,22 @@
         <v>27</v>
       </c>
       <c r="C8">
-        <v>0.03524002724002724</v>
+        <v>0.04366036603660365</v>
       </c>
       <c r="E8">
-        <v>-0.3040925920925922</v>
+        <v>-0.3633363336333633</v>
       </c>
       <c r="F8">
-        <v>0.4903575223575223</v>
+        <v>0.9007980798079807</v>
       </c>
       <c r="H8">
-        <v>0.9997759717759719</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="I8">
-        <v>0.7924959484959485</v>
+        <v>0.7969636963696368</v>
       </c>
       <c r="J8">
-        <v>-0.02086463484489577</v>
+        <v>-0.02724986110841934</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -682,22 +682,22 @@
         <v>28</v>
       </c>
       <c r="C9">
-        <v>0.964986796986797</v>
+        <v>0.9585118511851184</v>
       </c>
       <c r="E9">
-        <v>0.01353000153000153</v>
+        <v>0.04217221722172217</v>
       </c>
       <c r="F9">
-        <v>-0.01954833154833155</v>
+        <v>-0.001872187218721872</v>
       </c>
       <c r="H9">
-        <v>-0.0149016509016509</v>
+        <v>-0.0007320732073207321</v>
       </c>
       <c r="I9">
-        <v>-0.01146227946227946</v>
+        <v>0.1024542454245424</v>
       </c>
       <c r="J9">
-        <v>0.0221860640995974</v>
+        <v>-0.03904332237261846</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -708,22 +708,22 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>-0.00473905673905674</v>
+        <v>-0.09232523252325231</v>
       </c>
       <c r="E10">
-        <v>0.02764022764022764</v>
+        <v>-0.02384638463846384</v>
       </c>
       <c r="F10">
-        <v>-0.01215200415200415</v>
+        <v>0.05333333333333333</v>
       </c>
       <c r="H10">
-        <v>0.03131586731586732</v>
+        <v>0.05572157215721572</v>
       </c>
       <c r="I10">
-        <v>0.04357605157605158</v>
+        <v>-0.05666966696669666</v>
       </c>
       <c r="J10">
-        <v>0.01826569431243045</v>
+        <v>-0.03999808833036167</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -734,22 +734,22 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>-0.03709177309177309</v>
+        <v>-0.04882088208820882</v>
       </c>
       <c r="E11">
-        <v>-0.03686466086466087</v>
+        <v>0.1453585358535853</v>
       </c>
       <c r="F11">
-        <v>0.0350929070929071</v>
+        <v>-0.2312751275127513</v>
       </c>
       <c r="H11">
-        <v>-0.04453786453786453</v>
+        <v>-0.2049324932493249</v>
       </c>
       <c r="I11">
-        <v>-0.05375321375321376</v>
+        <v>-0.1155475547554755</v>
       </c>
       <c r="J11">
-        <v>-0.01477993000562896</v>
+        <v>0.08386928384779484</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -760,22 +760,22 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>0.05256611256611257</v>
+        <v>-0.004776477647764776</v>
       </c>
       <c r="E12">
-        <v>-0.02651784251784252</v>
+        <v>-0.05942994299429943</v>
       </c>
       <c r="F12">
-        <v>0.03053051453051453</v>
+        <v>-0.04667266726672666</v>
       </c>
       <c r="H12">
-        <v>-0.01388286188286188</v>
+        <v>-0.09008100810081007</v>
       </c>
       <c r="I12">
-        <v>-0.02742773142773143</v>
+        <v>-0.1073267326732673</v>
       </c>
       <c r="J12">
-        <v>-0.01184897533039653</v>
+        <v>-0.2109372236704616</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -784,22 +784,22 @@
         <v>31</v>
       </c>
       <c r="C13">
-        <v>0.1031496791496792</v>
+        <v>0.3011461146114611</v>
       </c>
       <c r="E13">
-        <v>-0.005206961206961207</v>
+        <v>0.134005400540054</v>
       </c>
       <c r="F13">
-        <v>0.003686595686595687</v>
+        <v>-0.1176837683768377</v>
       </c>
       <c r="H13">
-        <v>-0.01794496194496194</v>
+        <v>-0.02807080708070807</v>
       </c>
       <c r="I13">
-        <v>0.5802783162783164</v>
+        <v>0.564128412841284</v>
       </c>
       <c r="J13">
-        <v>0.01807563320419748</v>
+        <v>-0.08758026096657033</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -808,22 +808,22 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>-0.2292568092568093</v>
+        <v>-0.1467506750675067</v>
       </c>
       <c r="E14">
-        <v>0.003102279102279102</v>
+        <v>0.08987698769876985</v>
       </c>
       <c r="F14">
-        <v>-0.0103978183978184</v>
+        <v>0.01033303330333033</v>
       </c>
       <c r="H14">
-        <v>-0.02445218445218445</v>
+        <v>0.03169516951695169</v>
       </c>
       <c r="I14">
-        <v>-0.02457429657429657</v>
+        <v>-0.05876987698769877</v>
       </c>
       <c r="J14">
-        <v>0.04371730251872426</v>
+        <v>-0.07938368529160506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor refractor; more work on lipidcane2g
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Element</t>
   </si>
@@ -85,6 +85,24 @@
     <t>biorefinery</t>
   </si>
   <si>
+    <t>Stream-crude glycerol</t>
+  </si>
+  <si>
+    <t>Stream-pure glycerine</t>
+  </si>
+  <si>
+    <t>Stream-cellulase</t>
+  </si>
+  <si>
+    <t>Pretreatment reactor system</t>
+  </si>
+  <si>
+    <t>Pretreatment and saccharification</t>
+  </si>
+  <si>
+    <t>Cofermenation</t>
+  </si>
+  <si>
     <t>Cane lipid content [dry wt. %]</t>
   </si>
   <si>
@@ -113,6 +131,27 @@
   </si>
   <si>
     <t>IRR [%]</t>
+  </si>
+  <si>
+    <t>Price [USD/kg]</t>
+  </si>
+  <si>
+    <t>Cellulase loading [wt. % cellulose]</t>
+  </si>
+  <si>
+    <t>Base cost [million USD]</t>
+  </si>
+  <si>
+    <t>Glucose yield [%]</t>
+  </si>
+  <si>
+    <t>Xylose yield [%]</t>
+  </si>
+  <si>
+    <t>Glucose to ethanol yield [%]</t>
+  </si>
+  <si>
+    <t>Xylose to ethanol yield [%]</t>
   </si>
 </sst>
 </file>
@@ -470,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -557,121 +596,121 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C4">
-        <v>0.03895589558955895</v>
+        <v>-0.02121219675248787</v>
       </c>
       <c r="E4">
-        <v>-0.06773477347734773</v>
+        <v>0.01133214832528593</v>
       </c>
       <c r="F4">
-        <v>-0.006924692469246924</v>
+        <v>-0.01875564372622575</v>
       </c>
       <c r="H4">
-        <v>-0.06741074107410741</v>
+        <v>-0.01932827549313102</v>
       </c>
       <c r="I4">
-        <v>-0.01120912091209121</v>
+        <v>-0.01894716392588655</v>
       </c>
       <c r="J4">
-        <v>0.01022620393733763</v>
+        <v>0.01196679858300604</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C5">
-        <v>-0.1369216921692169</v>
+        <v>-0.01027079695483188</v>
       </c>
       <c r="E5">
-        <v>-0.01947794779477947</v>
+        <v>-0.002859720594388823</v>
       </c>
       <c r="F5">
-        <v>-0.06955895589558955</v>
+        <v>0.0004260152810406112</v>
       </c>
       <c r="H5">
-        <v>-0.06672667266726671</v>
+        <v>0.001045199177807967</v>
       </c>
       <c r="I5">
-        <v>-0.1615121512151215</v>
+        <v>-0.00162593900903756</v>
       </c>
       <c r="J5">
-        <v>-0.000492395022232346</v>
+        <v>0.007470819134243793</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C6">
-        <v>0.04655265526552655</v>
+        <v>0.005565642654625705</v>
       </c>
       <c r="E6">
-        <v>0.1524872487248725</v>
+        <v>-0.008901098468043937</v>
       </c>
       <c r="F6">
-        <v>-0.06835883588358835</v>
+        <v>-0.002212107448484297</v>
       </c>
       <c r="H6">
-        <v>-0.0144974497449745</v>
+        <v>-0.004335209549408381</v>
       </c>
       <c r="I6">
-        <v>-0.05526552655265525</v>
+        <v>-0.002647487913899516</v>
       </c>
       <c r="J6">
-        <v>-0.04121706625125394</v>
+        <v>-0.001052227878661404</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C7">
-        <v>-0.003708370837083708</v>
+        <v>0.003830104665204186</v>
       </c>
       <c r="E7">
-        <v>0.06589858985898589</v>
+        <v>-0.0119754650870186</v>
       </c>
       <c r="F7">
-        <v>-0.0287068706870687</v>
+        <v>0.004614277816571112</v>
       </c>
       <c r="H7">
-        <v>0.006540654065406539</v>
+        <v>0.00527321877092875</v>
       </c>
       <c r="I7">
-        <v>0.004116411641164116</v>
+        <v>-0.0005958812398352496</v>
       </c>
       <c r="J7">
-        <v>-0.02175545323838768</v>
+        <v>-0.01427097217562373</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C8">
-        <v>0.04366036603660365</v>
+        <v>0.1091581988623279</v>
       </c>
       <c r="E8">
-        <v>-0.3633363336333633</v>
+        <v>-0.0251881402075256</v>
       </c>
       <c r="F8">
-        <v>0.9007980798079807</v>
+        <v>0.9864043686721746</v>
       </c>
       <c r="H8">
-        <v>0.9999999999999999</v>
+        <v>0.999999703071988</v>
       </c>
       <c r="I8">
-        <v>0.7969636963696368</v>
+        <v>0.9576457947858317</v>
       </c>
       <c r="J8">
-        <v>-0.02724986110841934</v>
+        <v>-0.05232393255469991</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -679,25 +718,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C9">
-        <v>0.9585118511851184</v>
+        <v>0.9547143702525748</v>
       </c>
       <c r="E9">
-        <v>0.04217221722172217</v>
+        <v>0.02177359546294381</v>
       </c>
       <c r="F9">
-        <v>-0.001872187218721872</v>
+        <v>-0.02881871548874862</v>
       </c>
       <c r="H9">
-        <v>-0.0007320732073207321</v>
+        <v>-0.02724712131388485</v>
       </c>
       <c r="I9">
-        <v>0.1024542454245424</v>
+        <v>-0.02565199811407992</v>
       </c>
       <c r="J9">
-        <v>-0.03904332237261846</v>
+        <v>-0.0114884708325753</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -705,25 +744,25 @@
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C10">
-        <v>-0.09232523252325231</v>
+        <v>0.004275035115001404</v>
       </c>
       <c r="E10">
-        <v>-0.02384638463846384</v>
+        <v>-0.0302864602194584</v>
       </c>
       <c r="F10">
-        <v>0.05333333333333333</v>
+        <v>0.01230549783621991</v>
       </c>
       <c r="H10">
-        <v>0.05572157215721572</v>
+        <v>0.01120683712027348</v>
       </c>
       <c r="I10">
-        <v>-0.05666966696669666</v>
+        <v>0.007491558251662329</v>
       </c>
       <c r="J10">
-        <v>-0.03999808833036167</v>
+        <v>0.00678602765793675</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -731,25 +770,25 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C11">
-        <v>-0.04882088208820882</v>
+        <v>-0.002858188050327522</v>
       </c>
       <c r="E11">
-        <v>0.1453585358535853</v>
+        <v>0.01224121306564852</v>
       </c>
       <c r="F11">
-        <v>-0.2312751275127513</v>
+        <v>0.004479560723182428</v>
       </c>
       <c r="H11">
-        <v>-0.2049324932493249</v>
+        <v>0.005149690765987629</v>
       </c>
       <c r="I11">
-        <v>-0.1155475547554755</v>
+        <v>0.008194044615761783</v>
       </c>
       <c r="J11">
-        <v>0.08386928384779484</v>
+        <v>0.01332652281091606</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -757,80 +796,311 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C12">
-        <v>-0.004776477647764776</v>
+        <v>0.06794655343786213</v>
       </c>
       <c r="E12">
-        <v>-0.05942994299429943</v>
+        <v>0.0009608923584356942</v>
       </c>
       <c r="F12">
-        <v>-0.04667266726672666</v>
+        <v>0.02226205701848227</v>
       </c>
       <c r="H12">
-        <v>-0.09008100810081007</v>
+        <v>0.02384258332170333</v>
       </c>
       <c r="I12">
-        <v>-0.1073267326732673</v>
+        <v>0.02000939523237581</v>
       </c>
       <c r="J12">
-        <v>-0.2109372236704616</v>
+        <v>-0.003671776165935196</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C13">
-        <v>0.3011461146114611</v>
+        <v>0.1030724379788975</v>
       </c>
       <c r="E13">
-        <v>0.134005400540054</v>
+        <v>-3.0021025200841E-05</v>
       </c>
       <c r="F13">
-        <v>-0.1176837683768377</v>
+        <v>-0.01293443629337745</v>
       </c>
       <c r="H13">
-        <v>-0.02807080708070807</v>
+        <v>-0.01320797592031903</v>
       </c>
       <c r="I13">
-        <v>0.564128412841284</v>
+        <v>0.267955776926231</v>
       </c>
       <c r="J13">
-        <v>-0.08758026096657033</v>
+        <v>0.01693974752792456</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C14">
-        <v>-0.1467506750675067</v>
+        <v>-0.199130951997238</v>
       </c>
       <c r="E14">
-        <v>0.08987698769876985</v>
+        <v>0.004154904454196178</v>
       </c>
       <c r="F14">
-        <v>0.01033303330333033</v>
+        <v>0.02337183309487332</v>
       </c>
       <c r="H14">
-        <v>0.03169516951695169</v>
+        <v>0.02070701910028076</v>
       </c>
       <c r="I14">
-        <v>-0.05876987698769877</v>
+        <v>0.02607368293094731</v>
       </c>
       <c r="J14">
-        <v>-0.07938368529160506</v>
+        <v>0.003341824777071115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15">
+        <v>-0.0135902301756092</v>
+      </c>
+      <c r="E15">
+        <v>0.009334619989384799</v>
+      </c>
+      <c r="F15">
+        <v>-0.001652742786109711</v>
+      </c>
+      <c r="H15">
+        <v>0.002053032658121306</v>
+      </c>
+      <c r="I15">
+        <v>0.004215266088610644</v>
+      </c>
+      <c r="J15">
+        <v>-0.0145836245990908</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16">
+        <v>-0.005417894232715768</v>
+      </c>
+      <c r="E16">
+        <v>0.00741367450454698</v>
+      </c>
+      <c r="F16">
+        <v>0.02319113267164531</v>
+      </c>
+      <c r="H16">
+        <v>0.02683620145744805</v>
+      </c>
+      <c r="I16">
+        <v>0.02145504949820198</v>
+      </c>
+      <c r="J16">
+        <v>-0.003247869444108686</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17">
+        <v>0.00874159177366367</v>
+      </c>
+      <c r="E17">
+        <v>-0.006627397321095892</v>
+      </c>
+      <c r="F17">
+        <v>0.04133105925324237</v>
+      </c>
+      <c r="H17">
+        <v>0.04119099668763986</v>
+      </c>
+      <c r="I17">
+        <v>0.04796831395073255</v>
+      </c>
+      <c r="J17">
+        <v>0.02058471401919945</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>0.02785799487431979</v>
+      </c>
+      <c r="E18">
+        <v>0.002684852171394086</v>
+      </c>
+      <c r="F18">
+        <v>0.01331132270845291</v>
+      </c>
+      <c r="H18">
+        <v>0.01336800773472031</v>
+      </c>
+      <c r="I18">
+        <v>0.01683920947356838</v>
+      </c>
+      <c r="J18">
+        <v>0.003519364899805935</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <v>0.0113997099599884</v>
+      </c>
+      <c r="E19">
+        <v>0.01252524731700989</v>
+      </c>
+      <c r="F19">
+        <v>-0.001650367362014694</v>
+      </c>
+      <c r="H19">
+        <v>0.002070557554822302</v>
+      </c>
+      <c r="I19">
+        <v>0.004456985650279426</v>
+      </c>
+      <c r="J19">
+        <v>-0.02312707169414742</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20">
+        <v>0.009629132353165291</v>
+      </c>
+      <c r="E20">
+        <v>0.004898395491935819</v>
+      </c>
+      <c r="F20">
+        <v>0.0001707341828293673</v>
+      </c>
+      <c r="H20">
+        <v>-0.0006025162801006511</v>
+      </c>
+      <c r="I20">
+        <v>-0.001009648360385934</v>
+      </c>
+      <c r="J20">
+        <v>-0.005255548383826097</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>0.02412859286914371</v>
+      </c>
+      <c r="E21">
+        <v>-0.01265854485834179</v>
+      </c>
+      <c r="F21">
+        <v>0.02518422225536888</v>
+      </c>
+      <c r="H21">
+        <v>0.02411183280447331</v>
+      </c>
+      <c r="I21">
+        <v>0.02411104560444182</v>
+      </c>
+      <c r="J21">
+        <v>0.01942925905578899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22">
+        <v>0.01149286020371441</v>
+      </c>
+      <c r="E22">
+        <v>0.02069680690787228</v>
+      </c>
+      <c r="F22">
+        <v>-3.233904129356165E-05</v>
+      </c>
+      <c r="H22">
+        <v>-0.0007787600951504037</v>
+      </c>
+      <c r="I22">
+        <v>-0.0009385170615406823</v>
+      </c>
+      <c r="J22">
+        <v>-0.006837923689731783</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23">
+        <v>-0.008647588377903534</v>
+      </c>
+      <c r="E23">
+        <v>-0.008701865820074631</v>
+      </c>
+      <c r="F23">
+        <v>-0.007082371867294874</v>
+      </c>
+      <c r="H23">
+        <v>-0.008510149204405966</v>
+      </c>
+      <c r="I23">
+        <v>-0.01020257877610315</v>
+      </c>
+      <c r="J23">
+        <v>-0.002345641358777564</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
implement reduced chemicals system in lipidcane2g for speed up
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -599,22 +599,22 @@
         <v>29</v>
       </c>
       <c r="C4">
-        <v>-0.02121219675248787</v>
+        <v>-0.02110846634833865</v>
       </c>
       <c r="E4">
-        <v>0.01133214832528593</v>
+        <v>0.01298645735145829</v>
       </c>
       <c r="F4">
-        <v>-0.01875564372622575</v>
+        <v>0.01845237328209493</v>
       </c>
       <c r="H4">
-        <v>-0.01932827549313102</v>
+        <v>-0.01932192278887691</v>
       </c>
       <c r="I4">
         <v>-0.01894716392588655</v>
       </c>
       <c r="J4">
-        <v>0.01196679858300604</v>
+        <v>0.00912542055411643</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -623,22 +623,22 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <v>-0.01027079695483188</v>
+        <v>-0.01038802927952117</v>
       </c>
       <c r="E5">
-        <v>-0.002859720594388823</v>
+        <v>0.0008490873939634957</v>
       </c>
       <c r="F5">
-        <v>0.0004260152810406112</v>
+        <v>-0.0008634068505362739</v>
       </c>
       <c r="H5">
-        <v>0.001045199177807967</v>
+        <v>0.001045050665802027</v>
       </c>
       <c r="I5">
         <v>-0.00162593900903756</v>
       </c>
       <c r="J5">
-        <v>0.007470819134243793</v>
+        <v>-0.005236802687123067</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -647,22 +647,22 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>0.005565642654625705</v>
+        <v>0.005607882560315302</v>
       </c>
       <c r="E6">
-        <v>-0.008901098468043937</v>
+        <v>-0.01080562968022519</v>
       </c>
       <c r="F6">
-        <v>-0.002212107448484297</v>
+        <v>0.004349788397991535</v>
       </c>
       <c r="H6">
-        <v>-0.004335209549408381</v>
+        <v>-0.004340060909602436</v>
       </c>
       <c r="I6">
         <v>-0.002647487913899516</v>
       </c>
       <c r="J6">
-        <v>-0.001052227878661404</v>
+        <v>0.004516980638787003</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -671,22 +671,22 @@
         <v>32</v>
       </c>
       <c r="C7">
-        <v>0.003830104665204186</v>
+        <v>0.00371736101269444</v>
       </c>
       <c r="E7">
-        <v>-0.0119754650870186</v>
+        <v>-0.006509300324372012</v>
       </c>
       <c r="F7">
-        <v>0.004614277816571112</v>
+        <v>-0.005087259371490373</v>
       </c>
       <c r="H7">
-        <v>0.00527321877092875</v>
+        <v>0.00526512376260495</v>
       </c>
       <c r="I7">
         <v>-0.0005958812398352496</v>
       </c>
       <c r="J7">
-        <v>-0.01427097217562373</v>
+        <v>0.01708004907309691</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -695,22 +695,22 @@
         <v>33</v>
       </c>
       <c r="C8">
-        <v>0.1091581988623279</v>
+        <v>0.1006796693711868</v>
       </c>
       <c r="E8">
-        <v>-0.0251881402075256</v>
+        <v>-0.1291824037272961</v>
       </c>
       <c r="F8">
-        <v>0.9864043686721746</v>
+        <v>-0.9990109740724388</v>
       </c>
       <c r="H8">
-        <v>0.999999703071988</v>
+        <v>0.9999999321279971</v>
       </c>
       <c r="I8">
         <v>0.9576457947858317</v>
       </c>
       <c r="J8">
-        <v>-0.05232393255469991</v>
+        <v>-0.04652471361905297</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -721,22 +721,22 @@
         <v>34</v>
       </c>
       <c r="C9">
-        <v>0.9547143702525748</v>
+        <v>0.9555876790235071</v>
       </c>
       <c r="E9">
-        <v>0.02177359546294381</v>
+        <v>0.009469105242764208</v>
       </c>
       <c r="F9">
-        <v>-0.02881871548874862</v>
+        <v>0.02704875573795023</v>
       </c>
       <c r="H9">
-        <v>-0.02724712131388485</v>
+        <v>-0.02724844620993785</v>
       </c>
       <c r="I9">
         <v>-0.02565199811407992</v>
       </c>
       <c r="J9">
-        <v>-0.0114884708325753</v>
+        <v>-0.001473274547790203</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -747,22 +747,22 @@
         <v>34</v>
       </c>
       <c r="C10">
-        <v>0.004275035115001404</v>
+        <v>0.004201949160077966</v>
       </c>
       <c r="E10">
-        <v>-0.0302864602194584</v>
+        <v>-0.02559751465590058</v>
       </c>
       <c r="F10">
-        <v>0.01230549783621991</v>
+        <v>-0.01065525652221026</v>
       </c>
       <c r="H10">
-        <v>0.01120683712027348</v>
+        <v>0.01121473408058936</v>
       </c>
       <c r="I10">
         <v>0.007491558251662329</v>
       </c>
       <c r="J10">
-        <v>0.00678602765793675</v>
+        <v>0.009003673972347252</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -773,22 +773,22 @@
         <v>35</v>
       </c>
       <c r="C11">
-        <v>-0.002858188050327522</v>
+        <v>-0.002770926926837077</v>
       </c>
       <c r="E11">
-        <v>0.01224121306564852</v>
+        <v>0.01180795314431812</v>
       </c>
       <c r="F11">
-        <v>0.004479560723182428</v>
+        <v>-0.005739596005583839</v>
       </c>
       <c r="H11">
-        <v>0.005149690765987629</v>
+        <v>0.005149507405980296</v>
       </c>
       <c r="I11">
         <v>0.008194044615761783</v>
       </c>
       <c r="J11">
-        <v>0.01332652281091606</v>
+        <v>0.03298319604652162</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -799,22 +799,22 @@
         <v>36</v>
       </c>
       <c r="C12">
-        <v>0.06794655343786213</v>
+        <v>0.06583467911338714</v>
       </c>
       <c r="E12">
-        <v>0.0009608923584356942</v>
+        <v>0.005426115865044634</v>
       </c>
       <c r="F12">
-        <v>0.02226205701848227</v>
+        <v>-0.02376828920673157</v>
       </c>
       <c r="H12">
-        <v>0.02384258332170333</v>
+        <v>0.0238435650177426</v>
       </c>
       <c r="I12">
         <v>0.02000939523237581</v>
       </c>
       <c r="J12">
-        <v>-0.003671776165935196</v>
+        <v>0.005048352938450342</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -823,22 +823,22 @@
         <v>37</v>
       </c>
       <c r="C13">
-        <v>0.1030724379788975</v>
+        <v>0.1039959086718363</v>
       </c>
       <c r="E13">
-        <v>-3.0021025200841E-05</v>
+        <v>-0.007767489814699592</v>
       </c>
       <c r="F13">
-        <v>-0.01293443629337745</v>
+        <v>0.01314472449378898</v>
       </c>
       <c r="H13">
-        <v>-0.01320797592031903</v>
+        <v>-0.01319980689599227</v>
       </c>
       <c r="I13">
         <v>0.267955776926231</v>
       </c>
       <c r="J13">
-        <v>0.01693974752792456</v>
+        <v>-0.0005701241463470946</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -847,22 +847,22 @@
         <v>38</v>
       </c>
       <c r="C14">
-        <v>-0.199130951997238</v>
+        <v>-0.2008365560334622</v>
       </c>
       <c r="E14">
-        <v>0.004154904454196178</v>
+        <v>-0.006794817487792698</v>
       </c>
       <c r="F14">
-        <v>0.02337183309487332</v>
+        <v>-0.0204392476335699</v>
       </c>
       <c r="H14">
-        <v>0.02070701910028076</v>
+        <v>0.02071611538864461</v>
       </c>
       <c r="I14">
         <v>0.02607368293094731</v>
       </c>
       <c r="J14">
-        <v>0.003341824777071115</v>
+        <v>0.02110973848436875</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -873,22 +873,22 @@
         <v>39</v>
       </c>
       <c r="C15">
-        <v>-0.0135902301756092</v>
+        <v>-0.01358717593548704</v>
       </c>
       <c r="E15">
-        <v>0.009334619989384799</v>
+        <v>0.007514182764567309</v>
       </c>
       <c r="F15">
-        <v>-0.001652742786109711</v>
+        <v>-0.003017292696691707</v>
       </c>
       <c r="H15">
-        <v>0.002053032658121306</v>
+        <v>0.002034027633361105</v>
       </c>
       <c r="I15">
         <v>0.004215266088610644</v>
       </c>
       <c r="J15">
-        <v>-0.0145836245990908</v>
+        <v>0.009964063139056177</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -899,22 +899,22 @@
         <v>39</v>
       </c>
       <c r="C16">
-        <v>-0.005417894232715768</v>
+        <v>-0.005732050405282015</v>
       </c>
       <c r="E16">
-        <v>0.00741367450454698</v>
+        <v>0.02061093135243725</v>
       </c>
       <c r="F16">
-        <v>0.02319113267164531</v>
+        <v>-0.02791832166073286</v>
       </c>
       <c r="H16">
-        <v>0.02683620145744805</v>
+        <v>0.02683639825745593</v>
       </c>
       <c r="I16">
         <v>0.02145504949820198</v>
       </c>
       <c r="J16">
-        <v>-0.003247869444108686</v>
+        <v>-0.006952602142632662</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -925,22 +925,22 @@
         <v>39</v>
       </c>
       <c r="C17">
-        <v>0.00874159177366367</v>
+        <v>0.008226549065061961</v>
       </c>
       <c r="E17">
-        <v>-0.006627397321095892</v>
+        <v>-0.01961454337658173</v>
       </c>
       <c r="F17">
-        <v>0.04133105925324237</v>
+        <v>-0.04102408320896332</v>
       </c>
       <c r="H17">
-        <v>0.04119099668763986</v>
+        <v>0.04119682091187282</v>
       </c>
       <c r="I17">
         <v>0.04796831395073255</v>
       </c>
       <c r="J17">
-        <v>0.02058471401919945</v>
+        <v>-0.005043380102597345</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -949,22 +949,22 @@
         <v>40</v>
       </c>
       <c r="C18">
-        <v>0.02785799487431979</v>
+        <v>0.02770170610006824</v>
       </c>
       <c r="E18">
-        <v>0.002684852171394086</v>
+        <v>-0.007052324922092996</v>
       </c>
       <c r="F18">
-        <v>0.01331132270845291</v>
+        <v>-0.01366606067464243</v>
       </c>
       <c r="H18">
-        <v>0.01336800773472031</v>
+        <v>0.01337110843884434</v>
       </c>
       <c r="I18">
         <v>0.01683920947356838</v>
       </c>
       <c r="J18">
-        <v>0.003519364899805935</v>
+        <v>-0.01201817090873828</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -975,22 +975,22 @@
         <v>41</v>
       </c>
       <c r="C19">
-        <v>0.0113997099599884</v>
+        <v>0.0113806524232261</v>
       </c>
       <c r="E19">
-        <v>0.01252524731700989</v>
+        <v>0.008526018101040722</v>
       </c>
       <c r="F19">
-        <v>-0.001650367362014694</v>
+        <v>-0.002496572067862882</v>
       </c>
       <c r="H19">
-        <v>0.002070557554822302</v>
+        <v>0.002056993330279733</v>
       </c>
       <c r="I19">
         <v>0.004456985650279426</v>
       </c>
       <c r="J19">
-        <v>-0.02312707169414742</v>
+        <v>-0.02763781249191481</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1001,22 +1001,22 @@
         <v>42</v>
       </c>
       <c r="C20">
-        <v>0.009629132353165291</v>
+        <v>0.009769741446789656</v>
       </c>
       <c r="E20">
-        <v>0.004898395491935819</v>
+        <v>0.02642357990494319</v>
       </c>
       <c r="F20">
-        <v>0.0001707341828293673</v>
+        <v>-0.0001738172229526889</v>
       </c>
       <c r="H20">
-        <v>-0.0006025162801006511</v>
+        <v>-0.0005815046632601864</v>
       </c>
       <c r="I20">
         <v>-0.001009648360385934</v>
       </c>
       <c r="J20">
-        <v>-0.005255548383826097</v>
+        <v>0.001269696444360062</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1025,22 +1025,22 @@
         <v>43</v>
       </c>
       <c r="C21">
-        <v>0.02412859286914371</v>
+        <v>0.02399470425578816</v>
       </c>
       <c r="E21">
-        <v>-0.01265854485834179</v>
+        <v>-0.02289703637188145</v>
       </c>
       <c r="F21">
-        <v>0.02518422225536888</v>
+        <v>-0.02384739839389593</v>
       </c>
       <c r="H21">
-        <v>0.02411183280447331</v>
+        <v>0.02410911158836446</v>
       </c>
       <c r="I21">
         <v>0.02411104560444182</v>
       </c>
       <c r="J21">
-        <v>0.01942925905578899</v>
+        <v>-0.02232792274893487</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1051,22 +1051,22 @@
         <v>44</v>
       </c>
       <c r="C22">
-        <v>0.01149286020371441</v>
+        <v>0.01143177376927095</v>
       </c>
       <c r="E22">
-        <v>0.02069680690787228</v>
+        <v>0.01954322622172905</v>
       </c>
       <c r="F22">
-        <v>-3.233904129356165E-05</v>
+        <v>0.0004399732975989318</v>
       </c>
       <c r="H22">
-        <v>-0.0007787600951504037</v>
+        <v>-0.0007685764147430565</v>
       </c>
       <c r="I22">
         <v>-0.0009385170615406823</v>
       </c>
       <c r="J22">
-        <v>-0.006837923689731783</v>
+        <v>-0.009056289951286765</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1075,22 +1075,22 @@
         <v>45</v>
       </c>
       <c r="C23">
-        <v>-0.008647588377903534</v>
+        <v>-0.008521247668849907</v>
       </c>
       <c r="E23">
-        <v>-0.008701865820074631</v>
+        <v>-0.001891189899647596</v>
       </c>
       <c r="F23">
-        <v>-0.007082371867294874</v>
+        <v>0.009148773005950919</v>
       </c>
       <c r="H23">
-        <v>-0.008510149204405966</v>
+        <v>-0.008496730227869209</v>
       </c>
       <c r="I23">
         <v>-0.01020257877610315</v>
       </c>
       <c r="J23">
-        <v>-0.002345641358777564</v>
+        <v>0.0008275322108500017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move lime addition tank to not vaporize water; run evaluation with HXN ideal thermo
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -599,7 +599,7 @@
         <v>29</v>
       </c>
       <c r="C4">
-        <v>-0.02110846634833865</v>
+        <v>-0.02110517777220711</v>
       </c>
       <c r="E4">
         <v>0.01298645735145829</v>
@@ -608,13 +608,13 @@
         <v>0.01845237328209493</v>
       </c>
       <c r="H4">
-        <v>-0.01932192278887691</v>
+        <v>-0.01932204413288176</v>
       </c>
       <c r="I4">
         <v>-0.01894716392588655</v>
       </c>
       <c r="J4">
-        <v>0.00912542055411643</v>
+        <v>0.005298518211624132</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -623,7 +623,7 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <v>-0.01038802927952117</v>
+        <v>-0.01038435439937417</v>
       </c>
       <c r="E5">
         <v>0.0008490873939634957</v>
@@ -632,13 +632,13 @@
         <v>-0.0008634068505362739</v>
       </c>
       <c r="H5">
-        <v>0.001045050665802027</v>
+        <v>0.001044555689782227</v>
       </c>
       <c r="I5">
         <v>-0.00162593900903756</v>
       </c>
       <c r="J5">
-        <v>-0.005236802687123067</v>
+        <v>-0.0240587194032336</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -647,7 +647,7 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>0.005607882560315302</v>
+        <v>0.005599445407977816</v>
       </c>
       <c r="E6">
         <v>-0.01080562968022519</v>
@@ -656,13 +656,13 @@
         <v>0.004349788397991535</v>
       </c>
       <c r="H6">
-        <v>-0.004340060909602436</v>
+        <v>-0.00433904628556185</v>
       </c>
       <c r="I6">
         <v>-0.002647487913899516</v>
       </c>
       <c r="J6">
-        <v>0.004516980638787003</v>
+        <v>0.007944272400270062</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -671,7 +671,7 @@
         <v>32</v>
       </c>
       <c r="C7">
-        <v>0.00371736101269444</v>
+        <v>0.003709482100379283</v>
       </c>
       <c r="E7">
         <v>-0.006509300324372012</v>
@@ -680,13 +680,13 @@
         <v>-0.005087259371490373</v>
       </c>
       <c r="H7">
-        <v>0.00526512376260495</v>
+        <v>0.005263369362534773</v>
       </c>
       <c r="I7">
         <v>-0.0005958812398352496</v>
       </c>
       <c r="J7">
-        <v>0.01708004907309691</v>
+        <v>0.03091636404310185</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -695,7 +695,7 @@
         <v>33</v>
       </c>
       <c r="C8">
-        <v>0.1006796693711868</v>
+        <v>0.1003134614205384</v>
       </c>
       <c r="E8">
         <v>-0.1291824037272961</v>
@@ -704,13 +704,13 @@
         <v>-0.9990109740724388</v>
       </c>
       <c r="H8">
-        <v>0.9999999321279971</v>
+        <v>0.9999999260799969</v>
       </c>
       <c r="I8">
         <v>0.9576457947858317</v>
       </c>
       <c r="J8">
-        <v>-0.04652471361905297</v>
+        <v>-0.005078108643618663</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -721,7 +721,7 @@
         <v>34</v>
       </c>
       <c r="C9">
-        <v>0.9555876790235071</v>
+        <v>0.9556117012964678</v>
       </c>
       <c r="E9">
         <v>0.009469105242764208</v>
@@ -730,13 +730,13 @@
         <v>0.02704875573795023</v>
       </c>
       <c r="H9">
-        <v>-0.02724844620993785</v>
+        <v>-0.02724838803393552</v>
       </c>
       <c r="I9">
         <v>-0.02565199811407992</v>
       </c>
       <c r="J9">
-        <v>-0.001473274547790203</v>
+        <v>-0.01420375172972474</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -747,7 +747,7 @@
         <v>34</v>
       </c>
       <c r="C10">
-        <v>0.004201949160077966</v>
+        <v>0.004209853032394121</v>
       </c>
       <c r="E10">
         <v>-0.02559751465590058</v>
@@ -756,13 +756,13 @@
         <v>-0.01065525652221026</v>
       </c>
       <c r="H10">
-        <v>0.01121473408058936</v>
+        <v>0.01121331462453258</v>
       </c>
       <c r="I10">
         <v>0.007491558251662329</v>
       </c>
       <c r="J10">
-        <v>0.009003673972347252</v>
+        <v>0.0008725577868348304</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -773,7 +773,7 @@
         <v>35</v>
       </c>
       <c r="C11">
-        <v>-0.002770926926837077</v>
+        <v>-0.002767619438704777</v>
       </c>
       <c r="E11">
         <v>0.01180795314431812</v>
@@ -782,13 +782,13 @@
         <v>-0.005739596005583839</v>
       </c>
       <c r="H11">
-        <v>0.005149507405980296</v>
+        <v>0.005150281358011254</v>
       </c>
       <c r="I11">
         <v>0.008194044615761783</v>
       </c>
       <c r="J11">
-        <v>0.03298319604652162</v>
+        <v>-0.0131357627083223</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -799,7 +799,7 @@
         <v>36</v>
       </c>
       <c r="C12">
-        <v>0.06583467911338714</v>
+        <v>0.06583369319334771</v>
       </c>
       <c r="E12">
         <v>0.005426115865044634</v>
@@ -808,13 +808,13 @@
         <v>-0.02376828920673157</v>
       </c>
       <c r="H12">
-        <v>0.0238435650177426</v>
+        <v>0.02384368088974723</v>
       </c>
       <c r="I12">
         <v>0.02000939523237581</v>
       </c>
       <c r="J12">
-        <v>0.005048352938450342</v>
+        <v>0.005299909018230406</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -823,7 +823,7 @@
         <v>37</v>
       </c>
       <c r="C13">
-        <v>0.1039959086718363</v>
+        <v>0.1040556061782242</v>
       </c>
       <c r="E13">
         <v>-0.007767489814699592</v>
@@ -832,13 +832,13 @@
         <v>0.01314472449378898</v>
       </c>
       <c r="H13">
-        <v>-0.01319980689599227</v>
+        <v>-0.01319918164796726</v>
       </c>
       <c r="I13">
         <v>0.267955776926231</v>
       </c>
       <c r="J13">
-        <v>-0.0005701241463470946</v>
+        <v>-0.003690461918066865</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -847,7 +847,7 @@
         <v>38</v>
       </c>
       <c r="C14">
-        <v>-0.2008365560334622</v>
+        <v>-0.2009272996530919</v>
       </c>
       <c r="E14">
         <v>-0.006794817487792698</v>
@@ -856,13 +856,13 @@
         <v>-0.0204392476335699</v>
       </c>
       <c r="H14">
-        <v>0.02071611538864461</v>
+        <v>0.02071691545267662</v>
       </c>
       <c r="I14">
         <v>0.02607368293094731</v>
       </c>
       <c r="J14">
-        <v>0.02110973848436875</v>
+        <v>0.008379181160454727</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -873,7 +873,7 @@
         <v>39</v>
       </c>
       <c r="C15">
-        <v>-0.01358717593548704</v>
+        <v>-0.01358549516741981</v>
       </c>
       <c r="E15">
         <v>0.007514182764567309</v>
@@ -882,13 +882,13 @@
         <v>-0.003017292696691707</v>
       </c>
       <c r="H15">
-        <v>0.002034027633361105</v>
+        <v>0.00203412401736496</v>
       </c>
       <c r="I15">
         <v>0.004215266088610644</v>
       </c>
       <c r="J15">
-        <v>0.009964063139056177</v>
+        <v>0.002421837686559839</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -899,7 +899,7 @@
         <v>39</v>
       </c>
       <c r="C16">
-        <v>-0.005732050405282015</v>
+        <v>-0.00573481827739273</v>
       </c>
       <c r="E16">
         <v>0.02061093135243725</v>
@@ -908,13 +908,13 @@
         <v>-0.02791832166073286</v>
       </c>
       <c r="H16">
-        <v>0.02683639825745593</v>
+        <v>0.02683685982547439</v>
       </c>
       <c r="I16">
         <v>0.02145504949820198</v>
       </c>
       <c r="J16">
-        <v>-0.006952602142632662</v>
+        <v>0.005196766652402004</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -925,7 +925,7 @@
         <v>39</v>
       </c>
       <c r="C17">
-        <v>0.008226549065061961</v>
+        <v>0.008202958888118355</v>
       </c>
       <c r="E17">
         <v>-0.01961454337658173</v>
@@ -934,13 +934,13 @@
         <v>-0.04102408320896332</v>
       </c>
       <c r="H17">
-        <v>0.04119682091187282</v>
+        <v>0.04119785166391406</v>
       </c>
       <c r="I17">
         <v>0.04796831395073255</v>
       </c>
       <c r="J17">
-        <v>-0.005043380102597345</v>
+        <v>-0.007845941383957901</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -949,7 +949,7 @@
         <v>40</v>
       </c>
       <c r="C18">
-        <v>0.02770170610006824</v>
+        <v>0.02768330241933209</v>
       </c>
       <c r="E18">
         <v>-0.007052324922092996</v>
@@ -958,13 +958,13 @@
         <v>-0.01366606067464243</v>
       </c>
       <c r="H18">
-        <v>0.01337110843884434</v>
+        <v>0.01336923394276936</v>
       </c>
       <c r="I18">
         <v>0.01683920947356838</v>
       </c>
       <c r="J18">
-        <v>-0.01201817090873828</v>
+        <v>0.01234322590784038</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -975,7 +975,7 @@
         <v>41</v>
       </c>
       <c r="C19">
-        <v>0.0113806524232261</v>
+        <v>0.01138995165559806</v>
       </c>
       <c r="E19">
         <v>0.008526018101040722</v>
@@ -984,13 +984,13 @@
         <v>-0.002496572067862882</v>
       </c>
       <c r="H19">
-        <v>0.002056993330279733</v>
+        <v>0.002057256082290243</v>
       </c>
       <c r="I19">
         <v>0.004456985650279426</v>
       </c>
       <c r="J19">
-        <v>-0.02763781249191481</v>
+        <v>-0.01171673490626191</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1001,7 +1001,7 @@
         <v>42</v>
       </c>
       <c r="C20">
-        <v>0.009769741446789656</v>
+        <v>0.009783347815333913</v>
       </c>
       <c r="E20">
         <v>0.02642357990494319</v>
@@ -1010,13 +1010,13 @@
         <v>-0.0001738172229526889</v>
       </c>
       <c r="H20">
-        <v>-0.0005815046632601864</v>
+        <v>-0.0005815280872611235</v>
       </c>
       <c r="I20">
         <v>-0.001009648360385934</v>
       </c>
       <c r="J20">
-        <v>0.001269696444360062</v>
+        <v>-0.02955310253406249</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1025,7 +1025,7 @@
         <v>43</v>
       </c>
       <c r="C21">
-        <v>0.02399470425578816</v>
+        <v>0.02397830707113228</v>
       </c>
       <c r="E21">
         <v>-0.02289703637188145</v>
@@ -1034,13 +1034,13 @@
         <v>-0.02384739839389593</v>
       </c>
       <c r="H21">
-        <v>0.02410911158836446</v>
+        <v>0.02410917101236684</v>
       </c>
       <c r="I21">
         <v>0.02411104560444182</v>
       </c>
       <c r="J21">
-        <v>-0.02232792274893487</v>
+        <v>-0.01716372760577314</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1051,7 +1051,7 @@
         <v>44</v>
       </c>
       <c r="C22">
-        <v>0.01143177376927095</v>
+        <v>0.01142114109684564</v>
       </c>
       <c r="E22">
         <v>0.01954322622172905</v>
@@ -1060,13 +1060,13 @@
         <v>0.0004399732975989318</v>
       </c>
       <c r="H22">
-        <v>-0.0007685764147430565</v>
+        <v>-0.0007680211507208459</v>
       </c>
       <c r="I22">
         <v>-0.0009385170615406823</v>
       </c>
       <c r="J22">
-        <v>-0.009056289951286765</v>
+        <v>0.0228612576295299</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1075,7 +1075,7 @@
         <v>45</v>
       </c>
       <c r="C23">
-        <v>-0.008521247668849907</v>
+        <v>-0.008519305108772203</v>
       </c>
       <c r="E23">
         <v>-0.001891189899647596</v>
@@ -1084,13 +1084,13 @@
         <v>0.009148773005950919</v>
       </c>
       <c r="H23">
-        <v>-0.008496730227869209</v>
+        <v>-0.008496251379850054</v>
       </c>
       <c r="I23">
         <v>-0.01020257877610315</v>
       </c>
       <c r="J23">
-        <v>0.0008275322108500017</v>
+        <v>-0.001876748153259229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more work on lipidcane2g
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -599,22 +599,22 @@
         <v>29</v>
       </c>
       <c r="C4">
-        <v>-0.02110517777220711</v>
+        <v>-0.02110507534020301</v>
       </c>
       <c r="E4">
-        <v>0.01298645735145829</v>
+        <v>0.01299622419984897</v>
       </c>
       <c r="F4">
-        <v>0.01845237328209493</v>
+        <v>0.01845261203410448</v>
       </c>
       <c r="H4">
-        <v>-0.01932204413288176</v>
+        <v>-0.01932280886891235</v>
       </c>
       <c r="I4">
         <v>-0.01894716392588655</v>
       </c>
       <c r="J4">
-        <v>0.005298518211624132</v>
+        <v>-0.0002583969705665081</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -623,22 +623,22 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <v>-0.01038435439937417</v>
+        <v>-0.0103843876153755</v>
       </c>
       <c r="E5">
-        <v>0.0008490873939634957</v>
+        <v>0.0008820878752835149</v>
       </c>
       <c r="F5">
-        <v>-0.0008634068505362739</v>
+        <v>-0.0008629962585198503</v>
       </c>
       <c r="H5">
-        <v>0.001044555689782227</v>
+        <v>0.001044197129767885</v>
       </c>
       <c r="I5">
         <v>-0.00162593900903756</v>
       </c>
       <c r="J5">
-        <v>-0.0240587194032336</v>
+        <v>0.004634320760550871</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -647,22 +647,22 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>0.005599445407977816</v>
+        <v>0.005599665823986632</v>
       </c>
       <c r="E6">
-        <v>-0.01080562968022519</v>
+        <v>-0.01079733825589353</v>
       </c>
       <c r="F6">
-        <v>0.004349788397991535</v>
+        <v>0.00434991626999665</v>
       </c>
       <c r="H6">
-        <v>-0.00433904628556185</v>
+        <v>-0.004338794477551778</v>
       </c>
       <c r="I6">
         <v>-0.002647487913899516</v>
       </c>
       <c r="J6">
-        <v>0.007944272400270062</v>
+        <v>0.006102731144028873</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -671,22 +671,22 @@
         <v>32</v>
       </c>
       <c r="C7">
-        <v>0.003709482100379283</v>
+        <v>0.003708964084358563</v>
       </c>
       <c r="E7">
-        <v>-0.006509300324372012</v>
+        <v>-0.006502285796091431</v>
       </c>
       <c r="F7">
-        <v>-0.005087259371490373</v>
+        <v>-0.005087549291501971</v>
       </c>
       <c r="H7">
-        <v>0.005263369362534773</v>
+        <v>0.005263921650556866</v>
       </c>
       <c r="I7">
         <v>-0.0005958812398352496</v>
       </c>
       <c r="J7">
-        <v>0.03091636404310185</v>
+        <v>0.0178803832675434</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -695,22 +695,22 @@
         <v>33</v>
       </c>
       <c r="C8">
-        <v>0.1003134614205384</v>
+        <v>0.1003132927485317</v>
       </c>
       <c r="E8">
-        <v>-0.1291824037272961</v>
+        <v>-0.1291804318872173</v>
       </c>
       <c r="F8">
-        <v>-0.9990109740724388</v>
+        <v>-0.9990109868404393</v>
       </c>
       <c r="H8">
-        <v>0.9999999260799969</v>
+        <v>0.9999999263679969</v>
       </c>
       <c r="I8">
         <v>0.9576457947858317</v>
       </c>
       <c r="J8">
-        <v>-0.005078108643618663</v>
+        <v>-0.01327333373497799</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -721,22 +721,22 @@
         <v>34</v>
       </c>
       <c r="C9">
-        <v>0.9556117012964678</v>
+        <v>0.9556117589924702</v>
       </c>
       <c r="E9">
-        <v>0.009469105242764208</v>
+        <v>0.009484258075370322</v>
       </c>
       <c r="F9">
-        <v>0.02704875573795023</v>
+        <v>0.02704918293796731</v>
       </c>
       <c r="H9">
-        <v>-0.02724838803393552</v>
+        <v>-0.0272487874899515</v>
       </c>
       <c r="I9">
         <v>-0.02565199811407992</v>
       </c>
       <c r="J9">
-        <v>-0.01420375172972474</v>
+        <v>0.01514218753701872</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -747,22 +747,22 @@
         <v>34</v>
       </c>
       <c r="C10">
-        <v>0.004209853032394121</v>
+        <v>0.00420973351238934</v>
       </c>
       <c r="E10">
-        <v>-0.02559751465590058</v>
+        <v>-0.0256102650884106</v>
       </c>
       <c r="F10">
-        <v>-0.01065525652221026</v>
+        <v>-0.0106556674022267</v>
       </c>
       <c r="H10">
-        <v>0.01121331462453258</v>
+        <v>0.01121277203251088</v>
       </c>
       <c r="I10">
         <v>0.007491558251662329</v>
       </c>
       <c r="J10">
-        <v>0.0008725577868348304</v>
+        <v>0.004729352569465431</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -773,22 +773,22 @@
         <v>35</v>
       </c>
       <c r="C11">
-        <v>-0.002767619438704777</v>
+        <v>-0.002767640078705602</v>
       </c>
       <c r="E11">
-        <v>0.01180795314431812</v>
+        <v>0.01176585791063432</v>
       </c>
       <c r="F11">
-        <v>-0.005739596005583839</v>
+        <v>-0.005739736453589458</v>
       </c>
       <c r="H11">
-        <v>0.005150281358011254</v>
+        <v>0.005150287886011515</v>
       </c>
       <c r="I11">
         <v>0.008194044615761783</v>
       </c>
       <c r="J11">
-        <v>-0.0131357627083223</v>
+        <v>0.00938861510029193</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -799,22 +799,22 @@
         <v>36</v>
       </c>
       <c r="C12">
-        <v>0.06583369319334771</v>
+        <v>0.06583375242535008</v>
       </c>
       <c r="E12">
-        <v>0.005426115865044634</v>
+        <v>0.005407630680305227</v>
       </c>
       <c r="F12">
-        <v>-0.02376828920673157</v>
+        <v>-0.02376814040672561</v>
       </c>
       <c r="H12">
-        <v>0.02384368088974723</v>
+        <v>0.02384326789773071</v>
       </c>
       <c r="I12">
         <v>0.02000939523237581</v>
       </c>
       <c r="J12">
-        <v>0.005299909018230406</v>
+        <v>0.02053901750261387</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -823,22 +823,22 @@
         <v>37</v>
       </c>
       <c r="C13">
-        <v>0.1040556061782242</v>
+        <v>0.1040558466582338</v>
       </c>
       <c r="E13">
-        <v>-0.007767489814699592</v>
+        <v>-0.007785995351439813</v>
       </c>
       <c r="F13">
-        <v>0.01314472449378898</v>
+        <v>0.01314400084576003</v>
       </c>
       <c r="H13">
-        <v>-0.01319918164796726</v>
+        <v>-0.01319955268798211</v>
       </c>
       <c r="I13">
         <v>0.267955776926231</v>
       </c>
       <c r="J13">
-        <v>-0.003690461918066865</v>
+        <v>0.003063219359999851</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -847,22 +847,22 @@
         <v>38</v>
       </c>
       <c r="C14">
-        <v>-0.2009272996530919</v>
+        <v>-0.2009269572210783</v>
       </c>
       <c r="E14">
-        <v>-0.006794817487792698</v>
+        <v>-0.006815835248633409</v>
       </c>
       <c r="F14">
-        <v>-0.0204392476335699</v>
+        <v>-0.02043957432158297</v>
       </c>
       <c r="H14">
-        <v>0.02071691545267662</v>
+        <v>0.0207165825246633</v>
       </c>
       <c r="I14">
         <v>0.02607368293094731</v>
       </c>
       <c r="J14">
-        <v>0.008379181160454727</v>
+        <v>-0.0103139570346046</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -873,22 +873,22 @@
         <v>39</v>
       </c>
       <c r="C15">
-        <v>-0.01358549516741981</v>
+        <v>-0.01358543574341743</v>
       </c>
       <c r="E15">
-        <v>0.007514182764567309</v>
+        <v>0.007478063723122547</v>
       </c>
       <c r="F15">
-        <v>-0.003017292696691707</v>
+        <v>-0.003017578104703124</v>
       </c>
       <c r="H15">
-        <v>0.00203412401736496</v>
+        <v>0.002034005841360233</v>
       </c>
       <c r="I15">
         <v>0.004215266088610644</v>
       </c>
       <c r="J15">
-        <v>0.002421837686559839</v>
+        <v>-0.0226197537969832</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -899,22 +899,22 @@
         <v>39</v>
       </c>
       <c r="C16">
-        <v>-0.00573481827739273</v>
+        <v>-0.005735100517404021</v>
       </c>
       <c r="E16">
-        <v>0.02061093135243725</v>
+        <v>0.02060028216801129</v>
       </c>
       <c r="F16">
-        <v>-0.02791832166073286</v>
+        <v>-0.02791851894074076</v>
       </c>
       <c r="H16">
-        <v>0.02683685982547439</v>
+        <v>0.02683653131346125</v>
       </c>
       <c r="I16">
         <v>0.02145504949820198</v>
       </c>
       <c r="J16">
-        <v>0.005196766652402004</v>
+        <v>0.01892102930053914</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -925,22 +925,22 @@
         <v>39</v>
       </c>
       <c r="C17">
-        <v>0.008202958888118355</v>
+        <v>0.008202406696096266</v>
       </c>
       <c r="E17">
-        <v>-0.01961454337658173</v>
+        <v>-0.01957260606290424</v>
       </c>
       <c r="F17">
-        <v>-0.04102408320896332</v>
+        <v>-0.04102319741692789</v>
       </c>
       <c r="H17">
-        <v>0.04119785166391406</v>
+        <v>0.04119831812793272</v>
       </c>
       <c r="I17">
         <v>0.04796831395073255</v>
       </c>
       <c r="J17">
-        <v>-0.007845941383957901</v>
+        <v>-0.01581977773879409</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -949,22 +949,22 @@
         <v>40</v>
       </c>
       <c r="C18">
-        <v>0.02768330241933209</v>
+        <v>0.02768263992330559</v>
       </c>
       <c r="E18">
-        <v>-0.007052324922092996</v>
+        <v>-0.007037450393498015</v>
       </c>
       <c r="F18">
-        <v>-0.01366606067464243</v>
+        <v>-0.0136662976026519</v>
       </c>
       <c r="H18">
-        <v>0.01336923394276936</v>
+        <v>0.01336968072678723</v>
       </c>
       <c r="I18">
         <v>0.01683920947356838</v>
       </c>
       <c r="J18">
-        <v>0.01234322590784038</v>
+        <v>0.0037378436055706</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -975,22 +975,22 @@
         <v>41</v>
       </c>
       <c r="C19">
-        <v>0.01138995165559806</v>
+        <v>0.0113900300876012</v>
       </c>
       <c r="E19">
-        <v>0.008526018101040722</v>
+        <v>0.008551873398074934</v>
       </c>
       <c r="F19">
-        <v>-0.002496572067862882</v>
+        <v>-0.002496253155850126</v>
       </c>
       <c r="H19">
-        <v>0.002057256082290243</v>
+        <v>0.002057380306295212</v>
       </c>
       <c r="I19">
         <v>0.004456985650279426</v>
       </c>
       <c r="J19">
-        <v>-0.01171673490626191</v>
+        <v>0.007263896298911399</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1001,22 +1001,22 @@
         <v>42</v>
       </c>
       <c r="C20">
-        <v>0.009783347815333913</v>
+        <v>0.009783588487343538</v>
       </c>
       <c r="E20">
-        <v>0.02642357990494319</v>
+        <v>0.02644106198564248</v>
       </c>
       <c r="F20">
-        <v>-0.0001738172229526889</v>
+        <v>-0.000173226726929069</v>
       </c>
       <c r="H20">
-        <v>-0.0005815280872611235</v>
+        <v>-0.0005817705832708231</v>
       </c>
       <c r="I20">
         <v>-0.001009648360385934</v>
       </c>
       <c r="J20">
-        <v>-0.02955310253406249</v>
+        <v>-0.005287484288086148</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1025,22 +1025,22 @@
         <v>43</v>
       </c>
       <c r="C21">
-        <v>0.02397830707113228</v>
+        <v>0.02397818927912757</v>
       </c>
       <c r="E21">
-        <v>-0.02289703637188145</v>
+        <v>-0.02289423835576954</v>
       </c>
       <c r="F21">
-        <v>-0.02384739839389593</v>
+        <v>-0.0238473775618951</v>
       </c>
       <c r="H21">
-        <v>0.02410917101236684</v>
+        <v>0.02410961184438447</v>
       </c>
       <c r="I21">
         <v>0.02411104560444182</v>
       </c>
       <c r="J21">
-        <v>-0.01716372760577314</v>
+        <v>0.006818723469679011</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1051,22 +1051,22 @@
         <v>44</v>
       </c>
       <c r="C22">
-        <v>0.01142114109684564</v>
+        <v>0.01142120330484813</v>
       </c>
       <c r="E22">
-        <v>0.01954322622172905</v>
+        <v>0.01957146721485869</v>
       </c>
       <c r="F22">
-        <v>0.0004399732975989318</v>
+        <v>0.0004406947376277894</v>
       </c>
       <c r="H22">
-        <v>-0.0007680211507208459</v>
+        <v>-0.000767975550719022</v>
       </c>
       <c r="I22">
         <v>-0.0009385170615406823</v>
       </c>
       <c r="J22">
-        <v>0.0228612576295299</v>
+        <v>0.004971578136974088</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1075,22 +1075,22 @@
         <v>45</v>
       </c>
       <c r="C23">
-        <v>-0.008519305108772203</v>
+        <v>-0.008519180980767238</v>
       </c>
       <c r="E23">
-        <v>-0.001891189899647596</v>
+        <v>-0.001915117228604689</v>
       </c>
       <c r="F23">
-        <v>0.009148773005950919</v>
+        <v>0.009148524845940992</v>
       </c>
       <c r="H23">
-        <v>-0.008496251379850054</v>
+        <v>-0.00849640152385606</v>
       </c>
       <c r="I23">
         <v>-0.01020257877610315</v>
       </c>
       <c r="J23">
-        <v>-0.001876748153259229</v>
+        <v>0.003500357872446744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update agile system to new githube biosteam
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Element</t>
   </si>
@@ -118,6 +118,21 @@
     <t>Capacity [ton/hr]</t>
   </si>
   <si>
+    <t>Cane  PL [% lipid]</t>
+  </si>
+  <si>
+    <t>Sorghum  PL [% lipid]</t>
+  </si>
+  <si>
+    <t>Cane  FFA [% lipid]</t>
+  </si>
+  <si>
+    <t>Sorghum  FFA [% lipid]</t>
+  </si>
+  <si>
+    <t>TAG to  FFA conversion [% lipid]</t>
+  </si>
+  <si>
     <t>Price [USD/gal]</t>
   </si>
   <si>
@@ -142,10 +157,16 @@
     <t>Base cost [million USD]</t>
   </si>
   <si>
-    <t>Glucose yield [%]</t>
-  </si>
-  <si>
-    <t>Xylose yield [%]</t>
+    <t>Cane glucose yield [%]</t>
+  </si>
+  <si>
+    <t>Sorghum glucose yield [%]</t>
+  </si>
+  <si>
+    <t>Cane xylose yield [%]</t>
+  </si>
+  <si>
+    <t>Sorghum xylose yield [%]</t>
   </si>
   <si>
     <t>Glucose to ethanol yield [%]</t>
@@ -509,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -599,22 +620,22 @@
         <v>29</v>
       </c>
       <c r="C4">
-        <v>-0.02110507534020301</v>
+        <v>-0.0457941217941218</v>
       </c>
       <c r="E4">
-        <v>0.01299622419984897</v>
+        <v>0.019996495996496</v>
       </c>
       <c r="F4">
-        <v>0.01845261203410448</v>
+        <v>-0.02008796008796009</v>
       </c>
       <c r="H4">
-        <v>-0.01932280886891235</v>
+        <v>0.01999048399048399</v>
       </c>
       <c r="I4">
-        <v>-0.01894716392588655</v>
+        <v>0.03146466746466747</v>
       </c>
       <c r="J4">
-        <v>-0.0002583969705665081</v>
+        <v>-0.02100718790644551</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -623,22 +644,22 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <v>-0.0103843876153755</v>
+        <v>-0.01878983478983479</v>
       </c>
       <c r="E5">
-        <v>0.0008820878752835149</v>
+        <v>0.0001625881625881626</v>
       </c>
       <c r="F5">
-        <v>-0.0008629962585198503</v>
+        <v>-0.0001121281121281121</v>
       </c>
       <c r="H5">
-        <v>0.001044197129767885</v>
+        <v>0.0001695001695001695</v>
       </c>
       <c r="I5">
-        <v>-0.00162593900903756</v>
+        <v>-0.006816534816534816</v>
       </c>
       <c r="J5">
-        <v>0.004634320760550871</v>
+        <v>0.01604010538333952</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -647,22 +668,22 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>0.005599665823986632</v>
+        <v>0.05640534840534841</v>
       </c>
       <c r="E6">
-        <v>-0.01079733825589353</v>
+        <v>0.02170695370695371</v>
       </c>
       <c r="F6">
-        <v>0.00434991626999665</v>
+        <v>-0.02182041382041382</v>
       </c>
       <c r="H6">
-        <v>-0.004338794477551778</v>
+        <v>0.02172153372153372</v>
       </c>
       <c r="I6">
-        <v>-0.002647487913899516</v>
+        <v>0.03009468609468609</v>
       </c>
       <c r="J6">
-        <v>0.006102731144028873</v>
+        <v>-0.02530947494528765</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -671,22 +692,22 @@
         <v>32</v>
       </c>
       <c r="C7">
-        <v>0.003708964084358563</v>
+        <v>-0.04132368532368533</v>
       </c>
       <c r="E7">
-        <v>-0.006502285796091431</v>
+        <v>-0.06303267903267903</v>
       </c>
       <c r="F7">
-        <v>-0.005087549291501971</v>
+        <v>0.06334260334260335</v>
       </c>
       <c r="H7">
-        <v>0.005263921650556866</v>
+        <v>-0.06305139905139906</v>
       </c>
       <c r="I7">
-        <v>-0.0005958812398352496</v>
+        <v>-0.04742785142785143</v>
       </c>
       <c r="J7">
-        <v>0.0178803832675434</v>
+        <v>-0.00195742969036228</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -695,378 +716,372 @@
         <v>33</v>
       </c>
       <c r="C8">
-        <v>0.1003132927485317</v>
+        <v>0.1424291504291504</v>
       </c>
       <c r="E8">
-        <v>-0.1291804318872173</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>-0.9990109868404393</v>
+        <v>-0.999975951975952</v>
       </c>
       <c r="H8">
-        <v>0.9999999263679969</v>
+        <v>0.9999999639999642</v>
       </c>
       <c r="I8">
-        <v>0.9576457947858317</v>
+        <v>0.9574888414888415</v>
       </c>
       <c r="J8">
-        <v>-0.01327333373497799</v>
+        <v>0.05063386226839763</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C9">
-        <v>0.9556117589924702</v>
+        <v>0.01131731931731932</v>
       </c>
       <c r="E9">
-        <v>0.009484258075370322</v>
+        <v>0.03406911406911407</v>
       </c>
       <c r="F9">
-        <v>0.02704918293796731</v>
+        <v>-0.03392176592176592</v>
       </c>
       <c r="H9">
-        <v>-0.0272487874899515</v>
+        <v>0.03407127407127408</v>
       </c>
       <c r="I9">
-        <v>-0.02565199811407992</v>
+        <v>0.02799237999237999</v>
       </c>
       <c r="J9">
-        <v>0.01514218753701872</v>
+        <v>0.02725343907065175</v>
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10">
-        <v>0.00420973351238934</v>
+        <v>-0.005696309696309697</v>
       </c>
       <c r="E10">
-        <v>-0.0256102650884106</v>
+        <v>-0.07773961773961774</v>
       </c>
       <c r="F10">
-        <v>-0.0106556674022267</v>
+        <v>0.07746292146292147</v>
       </c>
       <c r="H10">
-        <v>0.01121277203251088</v>
+        <v>-0.07774360174360175</v>
       </c>
       <c r="I10">
-        <v>0.007491558251662329</v>
+        <v>-0.09330344130344131</v>
       </c>
       <c r="J10">
-        <v>0.004729352569465431</v>
+        <v>0.01245996404830096</v>
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11">
-        <v>-0.002767640078705602</v>
+        <v>-0.04428146028146029</v>
       </c>
       <c r="E11">
-        <v>0.01176585791063432</v>
+        <v>-0.0083002403002403</v>
       </c>
       <c r="F11">
-        <v>-0.005739736453589458</v>
+        <v>0.008151560151560152</v>
       </c>
       <c r="H11">
-        <v>0.005150287886011515</v>
+        <v>-0.008300432300432301</v>
       </c>
       <c r="I11">
-        <v>0.008194044615761783</v>
+        <v>-0.015003147003147</v>
       </c>
       <c r="J11">
-        <v>0.00938861510029193</v>
+        <v>-0.003550922920038042</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12">
-        <v>0.06583375242535008</v>
+        <v>-0.03647612447612448</v>
       </c>
       <c r="E12">
-        <v>0.005407630680305227</v>
+        <v>-0.05202814002814003</v>
       </c>
       <c r="F12">
-        <v>-0.02376814040672561</v>
+        <v>0.0522956802956803</v>
       </c>
       <c r="H12">
-        <v>0.02384326789773071</v>
+        <v>-0.05203163203163204</v>
       </c>
       <c r="I12">
-        <v>0.02000939523237581</v>
+        <v>-0.03115366315366316</v>
       </c>
       <c r="J12">
-        <v>0.02053901750261387</v>
+        <v>-0.02456545295131314</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13">
-        <v>0.1040558466582338</v>
+        <v>0.01766185766185767</v>
       </c>
       <c r="E13">
-        <v>-0.007785995351439813</v>
+        <v>0.01692438492438493</v>
       </c>
       <c r="F13">
-        <v>0.01314400084576003</v>
+        <v>-0.01683172083172083</v>
       </c>
       <c r="H13">
-        <v>-0.01319955268798211</v>
+        <v>0.01691950091950092</v>
       </c>
       <c r="I13">
-        <v>0.267955776926231</v>
+        <v>0.01915155115155116</v>
       </c>
       <c r="J13">
-        <v>0.003063219359999851</v>
+        <v>0.02423379662571144</v>
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14">
-        <v>-0.2009269572210783</v>
+        <v>0.9538661938661938</v>
       </c>
       <c r="E14">
-        <v>-0.006815835248633409</v>
+        <v>0.008535620535620536</v>
       </c>
       <c r="F14">
-        <v>-0.02043957432158297</v>
+        <v>-0.008332628332628333</v>
       </c>
       <c r="H14">
-        <v>0.0207165825246633</v>
+        <v>0.008535896535896537</v>
       </c>
       <c r="I14">
-        <v>0.02607368293094731</v>
+        <v>0.000481968481968482</v>
       </c>
       <c r="J14">
-        <v>-0.0103139570346046</v>
+        <v>0.02864564521658962</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C15">
-        <v>-0.01358543574341743</v>
+        <v>-0.017998625998626</v>
       </c>
       <c r="E15">
-        <v>0.007478063723122547</v>
+        <v>-0.05821592221592222</v>
       </c>
       <c r="F15">
-        <v>-0.003017578104703124</v>
+        <v>0.05854137454137455</v>
       </c>
       <c r="H15">
-        <v>0.002034005841360233</v>
+        <v>-0.05822542622542622</v>
       </c>
       <c r="I15">
-        <v>0.004215266088610644</v>
+        <v>-0.06471343671343671</v>
       </c>
       <c r="J15">
-        <v>-0.0226197537969832</v>
+        <v>-0.009114950808990817</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16">
-        <v>-0.005735100517404021</v>
+        <v>-0.04566963366963368</v>
       </c>
       <c r="E16">
-        <v>0.02060028216801129</v>
+        <v>0.0008050328050328052</v>
       </c>
       <c r="F16">
-        <v>-0.02791851894074076</v>
+        <v>-0.0007625047625047626</v>
       </c>
       <c r="H16">
-        <v>0.02683653131346125</v>
+        <v>0.0008063648063648065</v>
       </c>
       <c r="I16">
-        <v>0.02145504949820198</v>
+        <v>-0.01223472023472024</v>
       </c>
       <c r="J16">
-        <v>0.01892102930053914</v>
+        <v>-0.006768880779222662</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C17">
-        <v>0.008202406696096266</v>
+        <v>0.02980316980316981</v>
       </c>
       <c r="E17">
-        <v>-0.01957260606290424</v>
+        <v>0.001388941388941389</v>
       </c>
       <c r="F17">
-        <v>-0.04102319741692789</v>
+        <v>-0.001649041649041649</v>
       </c>
       <c r="H17">
-        <v>0.04119831812793272</v>
+        <v>0.001393573393573394</v>
       </c>
       <c r="I17">
-        <v>0.04796831395073255</v>
+        <v>0.002827226827226827</v>
       </c>
       <c r="J17">
-        <v>-0.01581977773879409</v>
+        <v>0.02855663320935464</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C18">
-        <v>0.02768263992330559</v>
+        <v>0.06757870357870359</v>
       </c>
       <c r="E18">
-        <v>-0.007037450393498015</v>
+        <v>-0.01604386004386004</v>
       </c>
       <c r="F18">
-        <v>-0.0136662976026519</v>
+        <v>0.01578008778008778</v>
       </c>
       <c r="H18">
-        <v>0.01336968072678723</v>
+        <v>-0.01605941205941206</v>
       </c>
       <c r="I18">
-        <v>0.01683920947356838</v>
+        <v>0.2669475509475509</v>
       </c>
       <c r="J18">
-        <v>0.0037378436055706</v>
+        <v>-0.06440020824631279</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C19">
-        <v>0.0113900300876012</v>
+        <v>-0.1772029772029772</v>
       </c>
       <c r="E19">
-        <v>0.008551873398074934</v>
+        <v>-0.005936885936885937</v>
       </c>
       <c r="F19">
-        <v>-0.002496253155850126</v>
+        <v>0.005878121878121879</v>
       </c>
       <c r="H19">
-        <v>0.002057380306295212</v>
+        <v>-0.005948309948309949</v>
       </c>
       <c r="I19">
-        <v>0.004456985650279426</v>
+        <v>-0.01395296595296595</v>
       </c>
       <c r="J19">
-        <v>0.007263896298911399</v>
+        <v>0.01443608824129558</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C20">
-        <v>0.009783588487343538</v>
+        <v>0.03733000933000933</v>
       </c>
       <c r="E20">
-        <v>0.02644106198564248</v>
+        <v>0.01528349128349128</v>
       </c>
       <c r="F20">
-        <v>-0.000173226726929069</v>
+        <v>-0.01508054708054708</v>
       </c>
       <c r="H20">
-        <v>-0.0005817705832708231</v>
+        <v>0.01528687528687529</v>
       </c>
       <c r="I20">
-        <v>-0.001009648360385934</v>
+        <v>0.007792087792087793</v>
       </c>
       <c r="J20">
-        <v>-0.005287484288086148</v>
+        <v>-0.01449498733099561</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21">
-        <v>0.02397818927912757</v>
+        <v>-0.01621440421440421</v>
       </c>
       <c r="E21">
-        <v>-0.02289423835576954</v>
+        <v>-0.006385542385542386</v>
       </c>
       <c r="F21">
-        <v>-0.0238473775618951</v>
+        <v>0.00628001428001428</v>
       </c>
       <c r="H21">
-        <v>0.02410961184438447</v>
+        <v>-0.006402822402822403</v>
       </c>
       <c r="I21">
-        <v>0.02411104560444182</v>
+        <v>0.007805047805047806</v>
       </c>
       <c r="J21">
-        <v>0.006818723469679011</v>
+        <v>-0.008049160044275059</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C22">
-        <v>0.01142120330484813</v>
+        <v>-0.03874053874053874</v>
       </c>
       <c r="E22">
-        <v>0.01957146721485869</v>
+        <v>0.0212016452016452</v>
       </c>
       <c r="F22">
-        <v>0.0004406947376277894</v>
+        <v>-0.02117104517104517</v>
       </c>
       <c r="H22">
-        <v>-0.000767975550719022</v>
+        <v>0.02120733320733321</v>
       </c>
       <c r="I22">
-        <v>-0.0009385170615406823</v>
+        <v>0.02314093114093114</v>
       </c>
       <c r="J22">
-        <v>0.004971578136974088</v>
+        <v>0.05318342261968982</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1075,32 +1090,206 @@
         <v>45</v>
       </c>
       <c r="C23">
-        <v>-0.008519180980767238</v>
+        <v>-0.0002599082599082599</v>
       </c>
       <c r="E23">
-        <v>-0.001915117228604689</v>
+        <v>0.01832031032031032</v>
       </c>
       <c r="F23">
-        <v>0.009148524845940992</v>
+        <v>-0.01811053811053811</v>
       </c>
       <c r="H23">
-        <v>-0.00849640152385606</v>
+        <v>0.01831781431781432</v>
       </c>
       <c r="I23">
-        <v>-0.01020257877610315</v>
+        <v>0.02651451851451852</v>
       </c>
       <c r="J23">
-        <v>0.003500357872446744</v>
+        <v>0.04281355679536454</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24">
+        <v>-0.06023988023988024</v>
+      </c>
+      <c r="E24">
+        <v>-0.04826037626037626</v>
+      </c>
+      <c r="F24">
+        <v>0.04823602823602824</v>
+      </c>
+      <c r="H24">
+        <v>-0.04826197226197226</v>
+      </c>
+      <c r="I24">
+        <v>-0.05307761307761308</v>
+      </c>
+      <c r="J24">
+        <v>0.03179095025918574</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25">
+        <v>-0.01068217068217068</v>
+      </c>
+      <c r="E25">
+        <v>-0.01335658935658936</v>
+      </c>
+      <c r="F25">
+        <v>0.01344988944988945</v>
+      </c>
+      <c r="H25">
+        <v>-0.01336598536598537</v>
+      </c>
+      <c r="I25">
+        <v>-0.01765396165396165</v>
+      </c>
+      <c r="J25">
+        <v>-0.01936455106773045</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26">
+        <v>0.07334904134904136</v>
+      </c>
+      <c r="E26">
+        <v>0.002503574503574503</v>
+      </c>
+      <c r="F26">
+        <v>-0.002510606510606511</v>
+      </c>
+      <c r="H26">
+        <v>0.002504726504726505</v>
+      </c>
+      <c r="I26">
+        <v>-0.0006616566616566617</v>
+      </c>
+      <c r="J26">
+        <v>-0.005515226472158199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27">
+        <v>-0.003782475782475783</v>
+      </c>
+      <c r="E27">
+        <v>-0.01176626376626377</v>
+      </c>
+      <c r="F27">
+        <v>0.01168215568215568</v>
+      </c>
+      <c r="H27">
+        <v>-0.01177585177585178</v>
+      </c>
+      <c r="I27">
+        <v>-0.01829105429105429</v>
+      </c>
+      <c r="J27">
+        <v>-0.01509734173565798</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28">
+        <v>0.004310884310884311</v>
+      </c>
+      <c r="E28">
+        <v>-0.02956675756675757</v>
+      </c>
+      <c r="F28">
+        <v>0.02966542166542167</v>
+      </c>
+      <c r="H28">
+        <v>-0.02957905757905758</v>
+      </c>
+      <c r="I28">
+        <v>-0.02736665136665137</v>
+      </c>
+      <c r="J28">
+        <v>-0.01227044357508311</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29">
+        <v>0.00501032901032901</v>
+      </c>
+      <c r="E29">
+        <v>-0.0005648885648885649</v>
+      </c>
+      <c r="F29">
+        <v>0.0004415044415044415</v>
+      </c>
+      <c r="H29">
+        <v>-0.000563988563988564</v>
+      </c>
+      <c r="I29">
+        <v>-0.01078780678780679</v>
+      </c>
+      <c r="J29">
+        <v>-0.067911749041345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30">
+        <v>-0.006028038028038028</v>
+      </c>
+      <c r="E30">
+        <v>0.02385085185085185</v>
+      </c>
+      <c r="F30">
+        <v>-0.0235977235977236</v>
+      </c>
+      <c r="H30">
+        <v>0.02383966783966784</v>
+      </c>
+      <c r="I30">
+        <v>0.02691687891687892</v>
+      </c>
+      <c r="J30">
+        <v>0.03711161942841879</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="C1:P1"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A4:A13"/>
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
make feedstocks more accurate; work on contours
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Element</t>
   </si>
@@ -70,7 +70,7 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Stream-sugarcane</t>
+    <t>biorefinery</t>
   </si>
   <si>
     <t>Stream-ethanol</t>
@@ -82,16 +82,13 @@
     <t>Stream-natural gas</t>
   </si>
   <si>
-    <t>biorefinery</t>
-  </si>
-  <si>
     <t>Stream-crude glycerol</t>
   </si>
   <si>
     <t>Stream-pure glycerine</t>
   </si>
   <si>
-    <t>Stream-cellulase</t>
+    <t>cellulase</t>
   </si>
   <si>
     <t>Pretreatment reactor system</t>
@@ -103,76 +100,82 @@
     <t>Cofermenation</t>
   </si>
   <si>
+    <t>lipidcane</t>
+  </si>
+  <si>
+    <t>lipidsorghum</t>
+  </si>
+  <si>
+    <t>Lipid retention [%]</t>
+  </si>
+  <si>
+    <t>Bagasse lipid extraction efficiency [%]</t>
+  </si>
+  <si>
+    <t>Capacity [ton/hr]</t>
+  </si>
+  <si>
+    <t>Price [USD/gal]</t>
+  </si>
+  <si>
+    <t>Price [USD/cf]</t>
+  </si>
+  <si>
+    <t>Electricity price [USD/kWh]</t>
+  </si>
+  <si>
+    <t>Operating days [day/yr]</t>
+  </si>
+  <si>
+    <t>IRR [%]</t>
+  </si>
+  <si>
+    <t>Price [USD/kg]</t>
+  </si>
+  <si>
+    <t>Cellulase loading [wt. % cellulose]</t>
+  </si>
+  <si>
+    <t>Base cost [million USD]</t>
+  </si>
+  <si>
+    <t>Cane glucose yield [%]</t>
+  </si>
+  <si>
+    <t>Sorghum glucose yield [%]</t>
+  </si>
+  <si>
+    <t>Cane xylose yield [%]</t>
+  </si>
+  <si>
+    <t>Sorghum xylose yield [%]</t>
+  </si>
+  <si>
+    <t>Glucose to ethanol yield [%]</t>
+  </si>
+  <si>
+    <t>Xylose to ethanol yield [%]</t>
+  </si>
+  <si>
+    <t>Cane  PL [% lipid]</t>
+  </si>
+  <si>
+    <t>Sorghum  PL [% lipid]</t>
+  </si>
+  <si>
+    <t>Cane  FFA [% lipid]</t>
+  </si>
+  <si>
+    <t>Sorghum  FFA [% lipid]</t>
+  </si>
+  <si>
     <t>Cane lipid content [dry wt. %]</t>
   </si>
   <si>
     <t>Relative sorghum lipid content [dry wt. %]</t>
   </si>
   <si>
-    <t>Lipid retention [%]</t>
-  </si>
-  <si>
-    <t>Bagasse lipid extraction efficiency [%]</t>
-  </si>
-  <si>
-    <t>Capacity [ton/hr]</t>
-  </si>
-  <si>
-    <t>Cane  PL [% lipid]</t>
-  </si>
-  <si>
-    <t>Sorghum  PL [% lipid]</t>
-  </si>
-  <si>
-    <t>Cane  FFA [% lipid]</t>
-  </si>
-  <si>
-    <t>Sorghum  FFA [% lipid]</t>
-  </si>
-  <si>
     <t>TAG to  FFA conversion [% lipid]</t>
-  </si>
-  <si>
-    <t>Price [USD/gal]</t>
-  </si>
-  <si>
-    <t>Price [USD/cf]</t>
-  </si>
-  <si>
-    <t>Electricity price [USD/kWh]</t>
-  </si>
-  <si>
-    <t>Operating days [day/yr]</t>
-  </si>
-  <si>
-    <t>IRR [%]</t>
-  </si>
-  <si>
-    <t>Price [USD/kg]</t>
-  </si>
-  <si>
-    <t>Cellulase loading [wt. % cellulose]</t>
-  </si>
-  <si>
-    <t>Base cost [million USD]</t>
-  </si>
-  <si>
-    <t>Cane glucose yield [%]</t>
-  </si>
-  <si>
-    <t>Sorghum glucose yield [%]</t>
-  </si>
-  <si>
-    <t>Cane xylose yield [%]</t>
-  </si>
-  <si>
-    <t>Sorghum xylose yield [%]</t>
-  </si>
-  <si>
-    <t>Glucose to ethanol yield [%]</t>
-  </si>
-  <si>
-    <t>Xylose to ethanol yield [%]</t>
   </si>
 </sst>
 </file>
@@ -617,169 +620,177 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>-0.04534907734907735</v>
+        <v>-0.004630936630936631</v>
       </c>
       <c r="E4">
-        <v>0.019996495996496</v>
+        <v>0.0281896601896602</v>
       </c>
       <c r="F4">
-        <v>-0.02005968805968806</v>
+        <v>-0.02635533835533836</v>
       </c>
       <c r="H4">
-        <v>0.01999341199341199</v>
+        <v>0.02663190263190263</v>
       </c>
       <c r="I4">
-        <v>0.03146466746466747</v>
+        <v>0.01902651102651103</v>
       </c>
       <c r="J4">
-        <v>0.02058866411469807</v>
+        <v>0.0464054046620302</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5">
-        <v>-0.0187053307053307</v>
+        <v>-0.00256005856005856</v>
       </c>
       <c r="E5">
-        <v>0.0001625881625881626</v>
+        <v>0.03390083790083791</v>
       </c>
       <c r="F5">
-        <v>-0.0001493761493761494</v>
+        <v>-0.03151455151455152</v>
       </c>
       <c r="H5">
-        <v>0.0001692601692601693</v>
+        <v>0.03171115971115971</v>
       </c>
       <c r="I5">
-        <v>-0.006816534816534816</v>
+        <v>0.0271995391995392</v>
       </c>
       <c r="J5">
-        <v>-0.0481217959889297</v>
+        <v>-0.05680830069122011</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>0.0571946971946972</v>
+        <v>0.1705067785067785</v>
       </c>
       <c r="E6">
-        <v>0.02170695370695371</v>
+        <v>0.9467454467454467</v>
       </c>
       <c r="F6">
-        <v>-0.02178621378621379</v>
+        <v>-0.999980847980848</v>
       </c>
       <c r="H6">
-        <v>0.02171052971052971</v>
+        <v>0.9999999879999882</v>
       </c>
       <c r="I6">
-        <v>0.03009468609468609</v>
+        <v>0.9576163776163775</v>
       </c>
       <c r="J6">
-        <v>-0.00115409435965108</v>
+        <v>0.02655547593667502</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7">
-        <v>-0.04073525273525273</v>
+        <v>0.9478386598386598</v>
       </c>
       <c r="E7">
-        <v>-0.06303267903267903</v>
+        <v>0.01391139791139791</v>
       </c>
       <c r="F7">
-        <v>0.06333509133509133</v>
+        <v>-0.00916038916038916</v>
       </c>
       <c r="H7">
-        <v>-0.06304071904071905</v>
+        <v>0.008856488856488858</v>
       </c>
       <c r="I7">
-        <v>-0.04742785142785143</v>
+        <v>0.01704668904668905</v>
       </c>
       <c r="J7">
-        <v>0.00767016630689323</v>
+        <v>0.02477148066876149</v>
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C8">
-        <v>0.1698824538824539</v>
+        <v>-0.0455989655989656</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.02185100185100185</v>
       </c>
       <c r="F8">
-        <v>-0.9999808599808599</v>
+        <v>-0.02174171774171774</v>
       </c>
       <c r="H8">
-        <v>0.9999999879999882</v>
+        <v>0.0217008457008457</v>
       </c>
       <c r="I8">
-        <v>0.9574888414888415</v>
+        <v>0.02262560262560263</v>
       </c>
       <c r="J8">
-        <v>0.0005223628968783183</v>
+        <v>-0.008258867150316431</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C9">
-        <v>0.01086141486141486</v>
+        <v>-0.01678513678513678</v>
       </c>
       <c r="E9">
-        <v>0.03406911406911407</v>
+        <v>-0.02244592644592645</v>
       </c>
       <c r="F9">
-        <v>-0.03394276594276595</v>
+        <v>0.02232523032523033</v>
       </c>
       <c r="H9">
-        <v>0.03406724206724207</v>
+        <v>-0.02201908601908602</v>
       </c>
       <c r="I9">
-        <v>0.02799237999237999</v>
+        <v>-0.02031891231891232</v>
       </c>
       <c r="J9">
-        <v>0.01992898738603721</v>
+        <v>-0.007223538642825336</v>
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C10">
-        <v>-0.01101248301248301</v>
+        <v>0.02872792072792073</v>
       </c>
       <c r="E10">
-        <v>-0.07773961773961774</v>
+        <v>-0.04119246519246519</v>
       </c>
       <c r="F10">
-        <v>0.07748584148584149</v>
+        <v>0.03997271197271197</v>
       </c>
       <c r="H10">
-        <v>-0.07774355374355375</v>
+        <v>-0.04006381606381607</v>
       </c>
       <c r="I10">
-        <v>-0.09330344130344131</v>
+        <v>-0.02584209784209784</v>
       </c>
       <c r="J10">
-        <v>0.006934504926312752</v>
+        <v>0.01774745442362583</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -788,22 +799,22 @@
         <v>36</v>
       </c>
       <c r="C11">
-        <v>-0.04584591384591385</v>
+        <v>0.1482367602367602</v>
       </c>
       <c r="E11">
-        <v>-0.0083002403002403</v>
+        <v>-0.03412591012591012</v>
       </c>
       <c r="F11">
-        <v>0.008163896163896166</v>
+        <v>0.04462370062370062</v>
       </c>
       <c r="H11">
-        <v>-0.008299496299496299</v>
+        <v>-0.04453835653835655</v>
       </c>
       <c r="I11">
-        <v>-0.015003147003147</v>
+        <v>0.2350591510591511</v>
       </c>
       <c r="J11">
-        <v>0.01034392362391858</v>
+        <v>0.0005326213801475394</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -812,484 +823,490 @@
         <v>37</v>
       </c>
       <c r="C12">
-        <v>-0.03705310905310906</v>
+        <v>-0.1569583809583809</v>
       </c>
       <c r="E12">
-        <v>-0.05202814002814003</v>
+        <v>-0.03182283182283183</v>
       </c>
       <c r="F12">
-        <v>0.05225762825762826</v>
+        <v>0.03753878553878554</v>
       </c>
       <c r="H12">
-        <v>-0.05202722802722803</v>
+        <v>-0.03738102138102138</v>
       </c>
       <c r="I12">
-        <v>-0.03115366315366316</v>
+        <v>-0.02596225396225397</v>
       </c>
       <c r="J12">
-        <v>-0.01941240606085285</v>
+        <v>0.04553524989558845</v>
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C13">
-        <v>0.01774080574080574</v>
+        <v>0.02529290529290529</v>
       </c>
       <c r="E13">
-        <v>0.01692438492438493</v>
+        <v>0.02286111486111486</v>
       </c>
       <c r="F13">
-        <v>-0.01683761283761284</v>
+        <v>-0.01048027048027048</v>
       </c>
       <c r="H13">
-        <v>0.01691886491886492</v>
+        <v>0.01011100611100611</v>
       </c>
       <c r="I13">
-        <v>0.01915155115155116</v>
+        <v>0.004987024987024987</v>
       </c>
       <c r="J13">
-        <v>0.01274006924037553</v>
+        <v>-0.09919973250941438</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14">
-        <v>0.9436007956007957</v>
+        <v>-0.02715901515901516</v>
       </c>
       <c r="E14">
-        <v>0.008535620535620536</v>
+        <v>0.03078531078531078</v>
       </c>
       <c r="F14">
-        <v>-0.008406032406032406</v>
+        <v>-0.04204209004209004</v>
       </c>
       <c r="H14">
-        <v>0.008536532536532537</v>
+        <v>0.04194325794325794</v>
       </c>
       <c r="I14">
-        <v>0.000481968481968482</v>
+        <v>0.02794845994845995</v>
       </c>
       <c r="J14">
-        <v>0.002539355327802522</v>
+        <v>0.05896886255267882</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>0.03730857730857731</v>
+      </c>
+      <c r="E15">
+        <v>-0.003542775542775543</v>
+      </c>
+      <c r="F15">
+        <v>-0.004507204507204507</v>
+      </c>
+      <c r="H15">
+        <v>0.004086604086604087</v>
+      </c>
+      <c r="I15">
+        <v>0.01412559812559813</v>
+      </c>
+      <c r="J15">
+        <v>0.0009967995742187717</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C15">
-        <v>-0.02147202947202947</v>
-      </c>
-      <c r="E15">
-        <v>-0.05821592221592222</v>
-      </c>
-      <c r="F15">
-        <v>0.05849036249036249</v>
-      </c>
-      <c r="H15">
-        <v>-0.05822072222072223</v>
-      </c>
-      <c r="I15">
-        <v>-0.06471343671343671</v>
-      </c>
-      <c r="J15">
-        <v>-0.001644138210598107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C16">
-        <v>-0.04650689850689851</v>
+        <v>0.01144121944121944</v>
       </c>
       <c r="E16">
-        <v>0.0008050328050328052</v>
+        <v>0.0064990864990865</v>
       </c>
       <c r="F16">
-        <v>-0.0007864447864447865</v>
+        <v>0.005299997299997301</v>
       </c>
       <c r="H16">
-        <v>0.0008034608034608035</v>
+        <v>-0.005060525060525061</v>
       </c>
       <c r="I16">
-        <v>-0.01223472023472024</v>
+        <v>-0.002670542670542671</v>
       </c>
       <c r="J16">
-        <v>0.04385307089362129</v>
+        <v>0.04115878810677757</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>-0.0007843567843567845</v>
+      </c>
+      <c r="E17">
+        <v>0.01074818274818275</v>
+      </c>
+      <c r="F17">
+        <v>0.003607959607959608</v>
+      </c>
+      <c r="H17">
+        <v>-0.003587031587031587</v>
+      </c>
+      <c r="I17">
+        <v>-0.009847689847689849</v>
+      </c>
+      <c r="J17">
+        <v>-0.00706735178446666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C17">
-        <v>0.044995544995545</v>
-      </c>
-      <c r="E17">
-        <v>0.001388941388941389</v>
-      </c>
-      <c r="F17">
-        <v>-0.001607077607077607</v>
-      </c>
-      <c r="H17">
-        <v>0.001391053391053391</v>
-      </c>
-      <c r="I17">
-        <v>0.002827226827226827</v>
-      </c>
-      <c r="J17">
-        <v>-6.538410111341721E-05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="C18">
-        <v>0.09147892347892349</v>
+        <v>0.0335925215925216</v>
       </c>
       <c r="E18">
-        <v>-0.01604386004386004</v>
+        <v>0.04089869289869291</v>
       </c>
       <c r="F18">
-        <v>0.01587068787068787</v>
+        <v>-0.0263951303951304</v>
       </c>
       <c r="H18">
-        <v>-0.01605245205245205</v>
+        <v>0.02656681456681457</v>
       </c>
       <c r="I18">
-        <v>0.2669475509475509</v>
+        <v>0.01689010089010089</v>
       </c>
       <c r="J18">
-        <v>-0.01756239336183911</v>
+        <v>-0.007913931742407261</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19">
+        <v>0.01747877347877348</v>
+      </c>
+      <c r="E19">
+        <v>-0.0398949278949279</v>
+      </c>
+      <c r="F19">
+        <v>0.02708049908049908</v>
+      </c>
+      <c r="H19">
+        <v>-0.02724714324714325</v>
+      </c>
+      <c r="I19">
+        <v>-0.02482634482634483</v>
+      </c>
+      <c r="J19">
+        <v>0.03266887942858353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C19">
-        <v>-0.1826485586485586</v>
-      </c>
-      <c r="E19">
-        <v>-0.005936885936885937</v>
-      </c>
-      <c r="F19">
-        <v>0.005851913851913853</v>
-      </c>
-      <c r="H19">
-        <v>-0.005942513942513943</v>
-      </c>
-      <c r="I19">
-        <v>-0.01395296595296595</v>
-      </c>
-      <c r="J19">
-        <v>0.004210133288099765</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C20">
-        <v>0.03681792081792082</v>
+        <v>-0.08501116901116902</v>
       </c>
       <c r="E20">
-        <v>0.01528349128349128</v>
+        <v>-0.09090657090657092</v>
       </c>
       <c r="F20">
-        <v>-0.01512372312372312</v>
+        <v>0.08585752985752985</v>
       </c>
       <c r="H20">
-        <v>0.01528855528855529</v>
+        <v>-0.08571216171216171</v>
       </c>
       <c r="I20">
-        <v>0.007792087792087793</v>
+        <v>-0.08057872457872459</v>
       </c>
       <c r="J20">
-        <v>0.01606437068894265</v>
+        <v>-0.04719504368321668</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C21">
-        <v>-0.01572747972747973</v>
+        <v>-0.01439030639030639</v>
       </c>
       <c r="E21">
-        <v>-0.006385542385542386</v>
+        <v>-0.02091636891636892</v>
       </c>
       <c r="F21">
-        <v>0.00627997827997828</v>
+        <v>0.01727020127020127</v>
       </c>
       <c r="H21">
-        <v>-0.006392730392730393</v>
+        <v>-0.01738354138354139</v>
       </c>
       <c r="I21">
-        <v>0.007805047805047806</v>
+        <v>-0.02576385776385776</v>
       </c>
       <c r="J21">
-        <v>-0.02106921439630787</v>
+        <v>0.04112679672544255</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22">
-        <v>-0.03646219246219246</v>
+        <v>0.02619135819135819</v>
       </c>
       <c r="E22">
-        <v>0.0212016452016452</v>
+        <v>0.05779521379521379</v>
       </c>
       <c r="F22">
-        <v>-0.02116788916788917</v>
+        <v>-0.05213140013140014</v>
       </c>
       <c r="H22">
-        <v>0.0211995691995692</v>
+        <v>0.05204831204831206</v>
       </c>
       <c r="I22">
-        <v>0.02314093114093114</v>
+        <v>0.0384011424011424</v>
       </c>
       <c r="J22">
-        <v>-0.0230177183650426</v>
+        <v>0.003681284089693573</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23">
-        <v>0.001943905943905944</v>
+        <v>-0.08392637992637993</v>
       </c>
       <c r="E23">
-        <v>0.01832031032031032</v>
+        <v>0.003636027636027636</v>
       </c>
       <c r="F23">
-        <v>-0.01812183012183012</v>
+        <v>0.005407349407349407</v>
       </c>
       <c r="H23">
-        <v>0.01831840231840232</v>
+        <v>-0.005610833610833611</v>
       </c>
       <c r="I23">
-        <v>0.02651451851451852</v>
+        <v>-0.001917109917109917</v>
       </c>
       <c r="J23">
-        <v>0.01186539144238359</v>
+        <v>-0.04804439714803977</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24">
-        <v>-0.06007113607113607</v>
+        <v>0.03855967455967457</v>
       </c>
       <c r="E24">
-        <v>-0.04826037626037626</v>
+        <v>-0.002082818082818083</v>
       </c>
       <c r="F24">
-        <v>0.04824622824622825</v>
+        <v>0.008751248751248752</v>
       </c>
       <c r="H24">
-        <v>-0.04826304026304026</v>
+        <v>-0.008842040842040842</v>
       </c>
       <c r="I24">
-        <v>-0.05307761307761308</v>
+        <v>-0.0100943620943621</v>
       </c>
       <c r="J24">
-        <v>0.02399188010635544</v>
+        <v>-0.02494444664343306</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C25">
-        <v>-0.01085860685860686</v>
+        <v>0.02240572640572641</v>
       </c>
       <c r="E25">
-        <v>-0.01335658935658936</v>
+        <v>-0.045997713997714</v>
       </c>
       <c r="F25">
-        <v>0.01344892944892945</v>
+        <v>0.03992459192459193</v>
       </c>
       <c r="H25">
-        <v>-0.01336491736491737</v>
+        <v>-0.03985056385056385</v>
       </c>
       <c r="I25">
-        <v>-0.01765396165396165</v>
+        <v>-0.02873820473820474</v>
       </c>
       <c r="J25">
-        <v>-0.005704058926320267</v>
+        <v>-0.0786949019673545</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C26">
-        <v>0.07221048021048021</v>
+        <v>-0.03641074841074841</v>
       </c>
       <c r="E26">
-        <v>0.002503574503574503</v>
+        <v>-0.04127377727377728</v>
       </c>
       <c r="F26">
-        <v>-0.002525438525438526</v>
+        <v>0.03761684561684562</v>
       </c>
       <c r="H26">
-        <v>0.002503634503634504</v>
+        <v>-0.03772057372057373</v>
       </c>
       <c r="I26">
-        <v>-0.0006616566616566617</v>
+        <v>-0.03225016425016425</v>
       </c>
       <c r="J26">
-        <v>0.003849281394027005</v>
+        <v>-0.002999415621655229</v>
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C27">
-        <v>-0.006264354264354266</v>
+        <v>-0.0005934005934005934</v>
       </c>
       <c r="E27">
-        <v>-0.01176626376626377</v>
+        <v>0.0151998871998872</v>
       </c>
       <c r="F27">
-        <v>0.01166152766152766</v>
+        <v>-0.03293592893592893</v>
       </c>
       <c r="H27">
-        <v>-0.01177103977103977</v>
+        <v>0.03295887295887296</v>
       </c>
       <c r="I27">
-        <v>-0.01829105429105429</v>
+        <v>0.03971495171495171</v>
       </c>
       <c r="J27">
-        <v>0.0488902697441396</v>
+        <v>-0.001792267762467795</v>
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C28">
-        <v>0.003176595176595177</v>
+        <v>0.03281122481122482</v>
       </c>
       <c r="E28">
-        <v>-0.02956675756675757</v>
+        <v>-0.001092853092853093</v>
       </c>
       <c r="F28">
-        <v>0.02967017367017367</v>
+        <v>0.002512574512574513</v>
       </c>
       <c r="H28">
-        <v>-0.02956945756945757</v>
+        <v>-0.002376242376242376</v>
       </c>
       <c r="I28">
-        <v>-0.02736665136665137</v>
+        <v>0.004126060126060127</v>
       </c>
       <c r="J28">
-        <v>-0.008927949936206599</v>
+        <v>-0.01308111914276333</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29">
-        <v>0.005491949491949492</v>
+        <v>-0.05194674394674396</v>
       </c>
       <c r="E29">
-        <v>-0.0005648885648885649</v>
+        <v>-0.03941289941289942</v>
       </c>
       <c r="F29">
-        <v>0.0004868404868404868</v>
+        <v>0.03683570483570484</v>
       </c>
       <c r="H29">
-        <v>-0.0005643005643005644</v>
+        <v>-0.03701690501690501</v>
       </c>
       <c r="I29">
-        <v>-0.01078780678780679</v>
+        <v>-0.03041409041409042</v>
       </c>
       <c r="J29">
-        <v>-0.02389354525792897</v>
+        <v>0.04409446709949042</v>
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C30">
-        <v>-0.004174660174660175</v>
+        <v>0.03025671025671026</v>
       </c>
       <c r="E30">
-        <v>0.02385085185085185</v>
+        <v>0.003998367998367999</v>
       </c>
       <c r="F30">
-        <v>-0.02365850365850366</v>
+        <v>-0.01442695442695443</v>
       </c>
       <c r="H30">
-        <v>0.02384813984813985</v>
+        <v>0.01403924603924604</v>
       </c>
       <c r="I30">
-        <v>0.02691687891687892</v>
+        <v>0.01143314343314343</v>
       </c>
       <c r="J30">
-        <v>0.03298304229416294</v>
+        <v>-0.03838956755310725</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="C1:P1"/>
-    <mergeCell ref="A4:A13"/>
-    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
BDO reactor fix to use maximum reactor volume to find number of reactors and better cost correlations
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>Element</t>
   </si>
@@ -100,6 +100,9 @@
     <t>Cofermenation</t>
   </si>
   <si>
+    <t>Cofermentation</t>
+  </si>
+  <si>
     <t>lipidcane</t>
   </si>
   <si>
@@ -157,16 +160,22 @@
     <t>Xylose to ethanol yield [%]</t>
   </si>
   <si>
-    <t>Cane  PL [% lipid]</t>
-  </si>
-  <si>
-    <t>Sorghum  PL [% lipid]</t>
-  </si>
-  <si>
-    <t>Cane  FFA [% lipid]</t>
-  </si>
-  <si>
-    <t>Sorghum  FFA [% lipid]</t>
+    <t>Titer [g/L]</t>
+  </si>
+  <si>
+    <t>Productivity [g/L]</t>
+  </si>
+  <si>
+    <t>Cane  PL content [% lipid]</t>
+  </si>
+  <si>
+    <t>Sorghum  PL content [% lipid]</t>
+  </si>
+  <si>
+    <t>Cane  FFA content [% lipid]</t>
+  </si>
+  <si>
+    <t>Sorghum  FFA content [% lipid]</t>
   </si>
   <si>
     <t>Cane lipid content [dry wt. %]</t>
@@ -533,7 +542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -620,73 +629,73 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4">
-        <v>-0.004630936630936631</v>
+        <v>0.02941480785370196</v>
       </c>
       <c r="E4">
-        <v>0.0281896601896602</v>
+        <v>-0.01912964278241069</v>
       </c>
       <c r="F4">
-        <v>-0.02635533835533836</v>
+        <v>0.009766497941624486</v>
       </c>
       <c r="H4">
-        <v>0.02663190263190263</v>
+        <v>-0.00977771644442911</v>
       </c>
       <c r="I4">
-        <v>0.01902651102651103</v>
+        <v>-0.0116191664047916</v>
       </c>
       <c r="J4">
-        <v>0.0464054046620302</v>
+        <v>0.02152759614383947</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5">
-        <v>-0.00256005856005856</v>
+        <v>-0.01353887738471934</v>
       </c>
       <c r="E5">
-        <v>0.03390083790083791</v>
+        <v>-0.002821238205309551</v>
       </c>
       <c r="F5">
-        <v>-0.03151455151455152</v>
+        <v>0.001024828756207189</v>
       </c>
       <c r="H5">
-        <v>0.03171115971115971</v>
+        <v>-0.001042236260559065</v>
       </c>
       <c r="I5">
-        <v>0.0271995391995392</v>
+        <v>-0.001179184794796199</v>
       </c>
       <c r="J5">
-        <v>-0.05680830069122011</v>
+        <v>-0.01540242923769734</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>0.1705067785067785</v>
+        <v>0.1740318450079612</v>
       </c>
       <c r="E6">
-        <v>0.9467454467454467</v>
+        <v>0.9272815973203993</v>
       </c>
       <c r="F6">
-        <v>-0.999980847980848</v>
+        <v>-0.9999804549951138</v>
       </c>
       <c r="H6">
-        <v>0.9999999879999882</v>
+        <v>0.999999992499998</v>
       </c>
       <c r="I6">
-        <v>0.9576163776163775</v>
+        <v>0.9576270249067561</v>
       </c>
       <c r="J6">
-        <v>0.02655547593667502</v>
+        <v>-8.5753682871736E-06</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -694,25 +703,25 @@
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7">
-        <v>0.9478386598386598</v>
+        <v>0.9489182777295695</v>
       </c>
       <c r="E7">
-        <v>0.01391139791139791</v>
+        <v>0.01701226175306544</v>
       </c>
       <c r="F7">
-        <v>-0.00916038916038916</v>
+        <v>-0.01348773337193334</v>
       </c>
       <c r="H7">
-        <v>0.008856488856488858</v>
+        <v>0.01357526289381572</v>
       </c>
       <c r="I7">
-        <v>0.01704668904668905</v>
+        <v>0.01047732411933103</v>
       </c>
       <c r="J7">
-        <v>0.02477148066876149</v>
+        <v>-0.009592183502200053</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -720,25 +729,25 @@
         <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8">
-        <v>-0.0455989655989656</v>
+        <v>-0.005972440493110123</v>
       </c>
       <c r="E8">
-        <v>0.02185100185100185</v>
+        <v>0.008232215058053764</v>
       </c>
       <c r="F8">
-        <v>-0.02174171774171774</v>
+        <v>0.0007258291814572954</v>
       </c>
       <c r="H8">
-        <v>0.0217008457008457</v>
+        <v>-0.0006583891645972911</v>
       </c>
       <c r="I8">
-        <v>0.02262560262560263</v>
+        <v>-0.003575954393988598</v>
       </c>
       <c r="J8">
-        <v>-0.008258867150316431</v>
+        <v>0.01288402186257568</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -746,25 +755,25 @@
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9">
-        <v>-0.01678513678513678</v>
+        <v>-0.01645494411373603</v>
       </c>
       <c r="E9">
-        <v>-0.02244592644592645</v>
+        <v>-0.003353726338431585</v>
       </c>
       <c r="F9">
-        <v>0.02232523032523033</v>
+        <v>-0.007404930351232588</v>
       </c>
       <c r="H9">
-        <v>-0.02201908601908602</v>
+        <v>0.007433580358395089</v>
       </c>
       <c r="I9">
-        <v>-0.02031891231891232</v>
+        <v>5.008951252237813E-05</v>
       </c>
       <c r="J9">
-        <v>-0.007223538642825336</v>
+        <v>-0.007726833043858143</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -772,73 +781,73 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10">
-        <v>0.02872792072792073</v>
+        <v>0.05060823815205953</v>
       </c>
       <c r="E10">
-        <v>-0.04119246519246519</v>
+        <v>0.05471604617901154</v>
       </c>
       <c r="F10">
-        <v>0.03997271197271197</v>
+        <v>-0.05419664704916175</v>
       </c>
       <c r="H10">
-        <v>-0.04006381606381607</v>
+        <v>0.05413969803492451</v>
       </c>
       <c r="I10">
-        <v>-0.02584209784209784</v>
+        <v>0.05932141033035258</v>
       </c>
       <c r="J10">
-        <v>0.01774745442362583</v>
+        <v>0.009904493342634945</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11">
-        <v>0.1482367602367602</v>
+        <v>0.1069269072317268</v>
       </c>
       <c r="E11">
-        <v>-0.03412591012591012</v>
+        <v>-0.01034597058649265</v>
       </c>
       <c r="F11">
-        <v>0.04462370062370062</v>
+        <v>0.01834578908644727</v>
       </c>
       <c r="H11">
-        <v>-0.04453835653835655</v>
+        <v>-0.01840795810198953</v>
       </c>
       <c r="I11">
-        <v>0.2350591510591511</v>
+        <v>0.2622912295728074</v>
       </c>
       <c r="J11">
-        <v>0.0005326213801475394</v>
+        <v>-0.023769125977717</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12">
-        <v>-0.1569583809583809</v>
+        <v>-0.2026175501543876</v>
       </c>
       <c r="E12">
-        <v>-0.03182283182283183</v>
+        <v>-0.01139146634786659</v>
       </c>
       <c r="F12">
-        <v>0.03753878553878554</v>
+        <v>0.01531990132997533</v>
       </c>
       <c r="H12">
-        <v>-0.03738102138102138</v>
+        <v>-0.01531608682902171</v>
       </c>
       <c r="I12">
-        <v>-0.02596225396225397</v>
+        <v>-0.009278277819569454</v>
       </c>
       <c r="J12">
-        <v>0.04553524989558845</v>
+        <v>0.009822843500256957</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -846,25 +855,25 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13">
-        <v>0.02529290529290529</v>
+        <v>0.01550475987618997</v>
       </c>
       <c r="E13">
-        <v>0.02286111486111486</v>
+        <v>0.00503084375771094</v>
       </c>
       <c r="F13">
-        <v>-0.01048027048027048</v>
+        <v>0.002771919692979923</v>
       </c>
       <c r="H13">
-        <v>0.01011100611100611</v>
+        <v>-0.002599334149833538</v>
       </c>
       <c r="I13">
-        <v>0.004987024987024987</v>
+        <v>-0.002487198621799656</v>
       </c>
       <c r="J13">
-        <v>-0.09919973250941438</v>
+        <v>0.03117335543751376</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -872,25 +881,25 @@
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14">
-        <v>-0.02715901515901516</v>
+        <v>0.008684382671095668</v>
       </c>
       <c r="E14">
-        <v>0.03078531078531078</v>
+        <v>-0.01503469725867431</v>
       </c>
       <c r="F14">
-        <v>-0.04204209004209004</v>
+        <v>-0.009845483461370865</v>
       </c>
       <c r="H14">
-        <v>0.04194325794325794</v>
+        <v>0.009872453468113366</v>
       </c>
       <c r="I14">
-        <v>0.02794845994845995</v>
+        <v>0.008973687743421936</v>
       </c>
       <c r="J14">
-        <v>0.05896886255267882</v>
+        <v>-0.02052399440975183</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -898,49 +907,49 @@
         <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15">
-        <v>0.03730857730857731</v>
+        <v>0.002055710013927503</v>
       </c>
       <c r="E15">
-        <v>-0.003542775542775543</v>
+        <v>0.01686455221613805</v>
       </c>
       <c r="F15">
-        <v>-0.004507204507204507</v>
+        <v>-0.02920891630222908</v>
       </c>
       <c r="H15">
-        <v>0.004086604086604087</v>
+        <v>0.02907422826855707</v>
       </c>
       <c r="I15">
-        <v>0.01412559812559813</v>
+        <v>0.03034157858539465</v>
       </c>
       <c r="J15">
-        <v>0.0009967995742187717</v>
+        <v>-0.006579688439123123</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16">
-        <v>0.01144121944121944</v>
+        <v>0.003007863751965938</v>
       </c>
       <c r="E16">
-        <v>0.0064990864990865</v>
+        <v>-0.00968640992160248</v>
       </c>
       <c r="F16">
-        <v>0.005299997299997301</v>
+        <v>0.02518965929741482</v>
       </c>
       <c r="H16">
-        <v>-0.005060525060525061</v>
+        <v>-0.0252606288151572</v>
       </c>
       <c r="I16">
-        <v>-0.002670542670542671</v>
+        <v>-0.01607945951986488</v>
       </c>
       <c r="J16">
-        <v>0.04115878810677757</v>
+        <v>-0.01546416018340198</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -948,25 +957,25 @@
         <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17">
-        <v>-0.0007843567843567845</v>
+        <v>0.003683102420775605</v>
       </c>
       <c r="E17">
-        <v>0.01074818274818275</v>
+        <v>0.001077483269370817</v>
       </c>
       <c r="F17">
-        <v>0.003607959607959608</v>
+        <v>-0.01070875017718754</v>
       </c>
       <c r="H17">
-        <v>-0.003587031587031587</v>
+        <v>0.01060242415060604</v>
       </c>
       <c r="I17">
-        <v>-0.009847689847689849</v>
+        <v>0.001017133754283439</v>
       </c>
       <c r="J17">
-        <v>-0.00706735178446666</v>
+        <v>0.01279853831731187</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -974,97 +983,97 @@
         <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18">
-        <v>0.0335925215925216</v>
+        <v>0.009939257484814371</v>
       </c>
       <c r="E18">
-        <v>0.04089869289869291</v>
+        <v>0.01604369051092263</v>
       </c>
       <c r="F18">
-        <v>-0.0263951303951304</v>
+        <v>-0.01246069211517303</v>
       </c>
       <c r="H18">
-        <v>0.02656681456681457</v>
+        <v>0.01244925611231403</v>
       </c>
       <c r="I18">
-        <v>0.01689010089010089</v>
+        <v>0.009544404886101221</v>
       </c>
       <c r="J18">
-        <v>-0.007913931742407261</v>
+        <v>0.02187544633850829</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19">
-        <v>0.01747877347877348</v>
+        <v>0.03152429138107284</v>
       </c>
       <c r="E19">
-        <v>-0.0398949278949279</v>
+        <v>-0.01140801735200434</v>
       </c>
       <c r="F19">
-        <v>0.02708049908049908</v>
+        <v>0.003143705285926321</v>
       </c>
       <c r="H19">
-        <v>-0.02724714324714325</v>
+        <v>-0.003341723335430833</v>
       </c>
       <c r="I19">
-        <v>-0.02482634482634483</v>
+        <v>-0.006618253654563414</v>
       </c>
       <c r="J19">
-        <v>0.03266887942858353</v>
+        <v>0.02099171666717349</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C20">
-        <v>-0.08501116901116902</v>
+        <v>0.001218132304533076</v>
       </c>
       <c r="E20">
-        <v>-0.09090657090657092</v>
+        <v>-0.01941311135327784</v>
       </c>
       <c r="F20">
-        <v>0.08585752985752985</v>
+        <v>0.02938678934669733</v>
       </c>
       <c r="H20">
-        <v>-0.08571216171216171</v>
+        <v>-0.02944831936207985</v>
       </c>
       <c r="I20">
-        <v>-0.08057872457872459</v>
+        <v>-0.03183967695991924</v>
       </c>
       <c r="J20">
-        <v>-0.04719504368321668</v>
+        <v>0.003944168907142948</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21">
-        <v>-0.01439030639030639</v>
+        <v>-0.01112019578004894</v>
       </c>
       <c r="E21">
-        <v>-0.02091636891636892</v>
+        <v>-0.02678605419651355</v>
       </c>
       <c r="F21">
-        <v>0.01727020127020127</v>
+        <v>0.02868533217133305</v>
       </c>
       <c r="H21">
-        <v>-0.01738354138354139</v>
+        <v>-0.02887138471784618</v>
       </c>
       <c r="I21">
-        <v>-0.02576385776385776</v>
+        <v>-0.03873141518285379</v>
       </c>
       <c r="J21">
-        <v>0.04112679672544255</v>
+        <v>0.02932160715811319</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1072,49 +1081,49 @@
         <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22">
-        <v>0.02619135819135819</v>
+        <v>-0.01374628693657174</v>
       </c>
       <c r="E22">
-        <v>0.05779521379521379</v>
+        <v>4.129951032487758E-05</v>
       </c>
       <c r="F22">
-        <v>-0.05213140013140014</v>
+        <v>0.001811719952929988</v>
       </c>
       <c r="H22">
-        <v>0.05204831204831206</v>
+        <v>-0.001984150996037749</v>
       </c>
       <c r="I22">
-        <v>0.0384011424011424</v>
+        <v>0.004501625625406406</v>
       </c>
       <c r="J22">
-        <v>0.003681284089693573</v>
+        <v>-0.009121589531929685</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23">
-        <v>-0.08392637992637993</v>
+        <v>-0.02715441978860494</v>
       </c>
       <c r="E23">
-        <v>0.003636027636027636</v>
+        <v>-0.02905618176404545</v>
       </c>
       <c r="F23">
-        <v>0.005407349407349407</v>
+        <v>0.02108617577154394</v>
       </c>
       <c r="H23">
-        <v>-0.005610833610833611</v>
+        <v>-0.02110525727631432</v>
       </c>
       <c r="I23">
-        <v>-0.001917109917109917</v>
+        <v>-0.02827631506907876</v>
       </c>
       <c r="J23">
-        <v>-0.04804439714803977</v>
+        <v>-0.02591206458928833</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1122,191 +1131,242 @@
         <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24">
-        <v>0.03855967455967457</v>
+        <v>-0.004212524553131138</v>
       </c>
       <c r="E24">
-        <v>-0.002082818082818083</v>
+        <v>-0.02371696192924048</v>
       </c>
       <c r="F24">
-        <v>0.008751248751248752</v>
+        <v>0.03356786339196585</v>
       </c>
       <c r="H24">
-        <v>-0.008842040842040842</v>
+        <v>-0.03380995445248861</v>
       </c>
       <c r="I24">
-        <v>-0.0100943620943621</v>
+        <v>-0.02136614634153658</v>
       </c>
       <c r="J24">
-        <v>-0.02494444664343306</v>
+        <v>0.01968961512747397</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C25">
-        <v>0.02240572640572641</v>
+        <v>-0.02208698802174701</v>
       </c>
       <c r="E25">
-        <v>-0.045997713997714</v>
+        <v>-0.002294646573661643</v>
       </c>
       <c r="F25">
-        <v>0.03992459192459193</v>
+        <v>0.004760446190111547</v>
       </c>
       <c r="H25">
-        <v>-0.03985056385056385</v>
+        <v>-0.004793546698386674</v>
       </c>
       <c r="I25">
-        <v>-0.02873820473820474</v>
+        <v>-0.01063446565861641</v>
       </c>
       <c r="J25">
-        <v>-0.0786949019673545</v>
+        <v>0.03237794405419208</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C26">
-        <v>-0.03641074841074841</v>
+        <v>-0.01951374337843585</v>
       </c>
       <c r="E26">
-        <v>-0.04127377727377728</v>
+        <v>-0.006935349233837308</v>
       </c>
       <c r="F26">
-        <v>0.03761684561684562</v>
+        <v>0.003691886422971605</v>
       </c>
       <c r="H26">
-        <v>-0.03772057372057373</v>
+        <v>-0.00367884991971248</v>
       </c>
       <c r="I26">
-        <v>-0.03225016425016425</v>
+        <v>0.001864071466017867</v>
       </c>
       <c r="J26">
-        <v>-0.002999415621655229</v>
+        <v>-0.04633925368647526</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C27">
-        <v>-0.0005934005934005934</v>
+        <v>-0.003142797785699446</v>
       </c>
       <c r="E27">
-        <v>0.0151998871998872</v>
+        <v>-0.02542533335633334</v>
       </c>
       <c r="F27">
-        <v>-0.03293592893592893</v>
+        <v>0.01774198193549548</v>
       </c>
       <c r="H27">
-        <v>0.03295887295887296</v>
+        <v>-0.01791548547887137</v>
       </c>
       <c r="I27">
-        <v>0.03971495171495171</v>
+        <v>-0.02613039653259913</v>
       </c>
       <c r="J27">
-        <v>-0.001792267762467795</v>
+        <v>0.01620433948026695</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C28">
-        <v>0.03281122481122482</v>
+        <v>0.05938487684621921</v>
       </c>
       <c r="E28">
-        <v>-0.001092853092853093</v>
+        <v>-0.01949829937457484</v>
       </c>
       <c r="F28">
-        <v>0.002512574512574513</v>
+        <v>0.0104162156040539</v>
       </c>
       <c r="H28">
-        <v>-0.002376242376242376</v>
+        <v>-0.0104739476184869</v>
       </c>
       <c r="I28">
-        <v>0.004126060126060127</v>
+        <v>-0.0048133692033423</v>
       </c>
       <c r="J28">
-        <v>-0.01308111914276333</v>
+        <v>-0.01669326753991083</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C29">
-        <v>-0.05194674394674396</v>
+        <v>-0.01184257796064449</v>
       </c>
       <c r="E29">
-        <v>-0.03941289941289942</v>
+        <v>0.01455647763911941</v>
       </c>
       <c r="F29">
-        <v>0.03683570483570484</v>
+        <v>0.001248730812182703</v>
       </c>
       <c r="H29">
-        <v>-0.03701690501690501</v>
+        <v>-0.001344609336152334</v>
       </c>
       <c r="I29">
-        <v>-0.03041409041409042</v>
+        <v>0.003953183488295872</v>
       </c>
       <c r="J29">
-        <v>0.04409446709949042</v>
+        <v>-0.01425650325372697</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30">
+        <v>-0.03624465756116439</v>
+      </c>
+      <c r="E30">
+        <v>-0.01560615540153885</v>
+      </c>
+      <c r="F30">
+        <v>0.02801751100437775</v>
+      </c>
+      <c r="H30">
+        <v>-0.02810288352572088</v>
+      </c>
+      <c r="I30">
+        <v>-0.0253442508360627</v>
+      </c>
+      <c r="J30">
+        <v>-0.002873680350950502</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31">
+        <v>-0.001529857882464471</v>
+      </c>
+      <c r="E31">
+        <v>0.004233539558384889</v>
+      </c>
+      <c r="F31">
+        <v>-0.003400446850111712</v>
+      </c>
+      <c r="H31">
+        <v>0.003449708362427091</v>
+      </c>
+      <c r="I31">
+        <v>0.008552372138093034</v>
+      </c>
+      <c r="J31">
+        <v>0.003247015777780447</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30">
-        <v>0.03025671025671026</v>
-      </c>
-      <c r="E30">
-        <v>0.003998367998367999</v>
-      </c>
-      <c r="F30">
-        <v>-0.01442695442695443</v>
-      </c>
-      <c r="H30">
-        <v>0.01403924603924604</v>
-      </c>
-      <c r="I30">
-        <v>0.01143314343314343</v>
-      </c>
-      <c r="J30">
-        <v>-0.03838956755310725</v>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32">
+        <v>-0.03115085128771283</v>
+      </c>
+      <c r="E32">
+        <v>0.008799450699862675</v>
+      </c>
+      <c r="F32">
+        <v>-0.009751983937995983</v>
+      </c>
+      <c r="H32">
+        <v>0.009643854910963727</v>
+      </c>
+      <c r="I32">
+        <v>0.009905729476432368</v>
+      </c>
+      <c r="J32">
+        <v>-0.008194478762290892</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add saccharification time to parameters
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Element</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Price [USD/kg]</t>
+  </si>
+  <si>
+    <t>Tau</t>
   </si>
   <si>
     <t>Cellulase loading [wt. % cellulose]</t>
@@ -542,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -632,22 +635,22 @@
         <v>31</v>
       </c>
       <c r="C4">
-        <v>0.02941480785370196</v>
+        <v>-0.02283115780924631</v>
       </c>
       <c r="E4">
-        <v>-0.01912964278241069</v>
+        <v>0.03252158606886344</v>
       </c>
       <c r="F4">
-        <v>0.009766497941624486</v>
+        <v>-0.02345721060228842</v>
       </c>
       <c r="H4">
-        <v>-0.00977771644442911</v>
+        <v>0.02341656535266261</v>
       </c>
       <c r="I4">
-        <v>-0.0116191664047916</v>
+        <v>0.01824716780188671</v>
       </c>
       <c r="J4">
-        <v>0.02152759614383947</v>
+        <v>-0.01001126144342611</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -656,22 +659,22 @@
         <v>32</v>
       </c>
       <c r="C5">
-        <v>-0.01353887738471934</v>
+        <v>0.007191296927651877</v>
       </c>
       <c r="E5">
-        <v>-0.002821238205309551</v>
+        <v>0.0294076926963077</v>
       </c>
       <c r="F5">
-        <v>0.001024828756207189</v>
+        <v>-0.02395886351835454</v>
       </c>
       <c r="H5">
-        <v>-0.001042236260559065</v>
+        <v>0.02398984742359389</v>
       </c>
       <c r="I5">
-        <v>-0.001179184794796199</v>
+        <v>0.02099920672796826</v>
       </c>
       <c r="J5">
-        <v>-0.01540242923769734</v>
+        <v>0.009471818331361903</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -680,22 +683,22 @@
         <v>33</v>
       </c>
       <c r="C6">
-        <v>0.1740318450079612</v>
+        <v>0.1519870517114821</v>
       </c>
       <c r="E6">
-        <v>0.9272815973203993</v>
+        <v>0.9382294163451764</v>
       </c>
       <c r="F6">
-        <v>-0.9999804549951138</v>
+        <v>-0.9999804825272192</v>
       </c>
       <c r="H6">
-        <v>0.999999992499998</v>
+        <v>0.9999999916479996</v>
       </c>
       <c r="I6">
-        <v>0.9576270249067561</v>
+        <v>0.9586914095476562</v>
       </c>
       <c r="J6">
-        <v>-8.5753682871736E-06</v>
+        <v>-0.002172398423935881</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -706,22 +709,22 @@
         <v>34</v>
       </c>
       <c r="C7">
-        <v>0.9489182777295695</v>
+        <v>0.9484030940321236</v>
       </c>
       <c r="E7">
-        <v>0.01701226175306544</v>
+        <v>-0.01072744132509765</v>
       </c>
       <c r="F7">
-        <v>-0.01348773337193334</v>
+        <v>0.004923681892947275</v>
       </c>
       <c r="H7">
-        <v>0.01357526289381572</v>
+        <v>-0.004825162561006502</v>
       </c>
       <c r="I7">
-        <v>0.01047732411933103</v>
+        <v>0.002488744899549796</v>
       </c>
       <c r="J7">
-        <v>-0.009592183502200053</v>
+        <v>0.007057077690483055</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -732,22 +735,22 @@
         <v>34</v>
       </c>
       <c r="C8">
-        <v>-0.005972440493110123</v>
+        <v>0.0225188151727526</v>
       </c>
       <c r="E8">
-        <v>0.008232215058053764</v>
+        <v>0.01356077353443094</v>
       </c>
       <c r="F8">
-        <v>0.0007258291814572954</v>
+        <v>-0.01314891086195643</v>
       </c>
       <c r="H8">
-        <v>-0.0006583891645972911</v>
+        <v>0.01312995364519814</v>
       </c>
       <c r="I8">
-        <v>-0.003575954393988598</v>
+        <v>0.01808265845130633</v>
       </c>
       <c r="J8">
-        <v>0.01288402186257568</v>
+        <v>0.01109177598846261</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -758,22 +761,22 @@
         <v>35</v>
       </c>
       <c r="C9">
-        <v>-0.01645494411373603</v>
+        <v>-0.004604815384192615</v>
       </c>
       <c r="E9">
-        <v>-0.003353726338431585</v>
+        <v>-0.007437114921484595</v>
       </c>
       <c r="F9">
-        <v>-0.007404930351232588</v>
+        <v>0.01417645611905824</v>
       </c>
       <c r="H9">
-        <v>0.007433580358395089</v>
+        <v>-0.01424939039397561</v>
       </c>
       <c r="I9">
-        <v>5.008951252237813E-05</v>
+        <v>-0.0166405299776212</v>
       </c>
       <c r="J9">
-        <v>-0.007726833043858143</v>
+        <v>-0.01220219018234914</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -784,22 +787,22 @@
         <v>36</v>
       </c>
       <c r="C10">
-        <v>0.05060823815205953</v>
+        <v>0.04784935650597425</v>
       </c>
       <c r="E10">
-        <v>0.05471604617901154</v>
+        <v>0.02169796397191855</v>
       </c>
       <c r="F10">
-        <v>-0.05419664704916175</v>
+        <v>-0.01818195691927827</v>
       </c>
       <c r="H10">
-        <v>0.05413969803492451</v>
+        <v>0.01806241377849655</v>
       </c>
       <c r="I10">
-        <v>0.05932141033035258</v>
+        <v>0.01400161121606445</v>
       </c>
       <c r="J10">
-        <v>0.009904493342634945</v>
+        <v>0.006567211724689074</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -808,22 +811,22 @@
         <v>37</v>
       </c>
       <c r="C11">
-        <v>0.1069269072317268</v>
+        <v>0.1444172317606893</v>
       </c>
       <c r="E11">
-        <v>-0.01034597058649265</v>
+        <v>0.003330341797213672</v>
       </c>
       <c r="F11">
-        <v>0.01834578908644727</v>
+        <v>-0.007889097819563913</v>
       </c>
       <c r="H11">
-        <v>-0.01840795810198953</v>
+        <v>0.007686511507460459</v>
       </c>
       <c r="I11">
-        <v>0.2622912295728074</v>
+        <v>0.283372950726918</v>
       </c>
       <c r="J11">
-        <v>-0.023769125977717</v>
+        <v>-0.005271696816414461</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -832,22 +835,22 @@
         <v>38</v>
       </c>
       <c r="C12">
-        <v>-0.2026175501543876</v>
+        <v>-0.1937698121987924</v>
       </c>
       <c r="E12">
-        <v>-0.01139146634786659</v>
+        <v>0.01269399737175989</v>
       </c>
       <c r="F12">
-        <v>0.01531990132997533</v>
+        <v>-0.01446597360263894</v>
       </c>
       <c r="H12">
-        <v>-0.01531608682902171</v>
+        <v>0.01444677158587086</v>
       </c>
       <c r="I12">
-        <v>-0.009278277819569454</v>
+        <v>0.01842309193692368</v>
       </c>
       <c r="J12">
-        <v>0.009822843500256957</v>
+        <v>-0.003221754185824128</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -858,22 +861,22 @@
         <v>39</v>
       </c>
       <c r="C13">
-        <v>0.01550475987618997</v>
+        <v>0.02240781219231248</v>
       </c>
       <c r="E13">
-        <v>0.00503084375771094</v>
+        <v>-0.001322413396896536</v>
       </c>
       <c r="F13">
-        <v>0.002771919692979923</v>
+        <v>0.00466661701866468</v>
       </c>
       <c r="H13">
-        <v>-0.002599334149833538</v>
+        <v>-0.00473076825323073</v>
       </c>
       <c r="I13">
-        <v>-0.002487198621799656</v>
+        <v>-0.004888350915534036</v>
       </c>
       <c r="J13">
-        <v>0.03117335543751376</v>
+        <v>0.01383563057094249</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -884,148 +887,150 @@
         <v>39</v>
       </c>
       <c r="C14">
-        <v>0.008684382671095668</v>
+        <v>5.901744236069768E-05</v>
       </c>
       <c r="E14">
-        <v>-0.01503469725867431</v>
+        <v>-0.005465977850639113</v>
       </c>
       <c r="F14">
-        <v>-0.009845483461370865</v>
+        <v>0.0001964740878589635</v>
       </c>
       <c r="H14">
-        <v>0.009872453468113366</v>
+        <v>-0.0001528324861132994</v>
       </c>
       <c r="I14">
-        <v>0.008973687743421936</v>
+        <v>-0.009953175374127014</v>
       </c>
       <c r="J14">
-        <v>-0.02052399440975183</v>
+        <v>-0.0006871099755667106</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>-0.01752631202905248</v>
+      </c>
+      <c r="E15">
+        <v>-0.007758804982352198</v>
+      </c>
+      <c r="F15">
+        <v>0.007814835000593398</v>
+      </c>
+      <c r="H15">
+        <v>-0.007782896567315861</v>
+      </c>
+      <c r="I15">
+        <v>-0.007891357275654291</v>
+      </c>
+      <c r="J15">
+        <v>0.02159517101128804</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C15">
-        <v>0.002055710013927503</v>
-      </c>
-      <c r="E15">
-        <v>0.01686455221613805</v>
-      </c>
-      <c r="F15">
-        <v>-0.02920891630222908</v>
-      </c>
-      <c r="H15">
-        <v>0.02907422826855707</v>
-      </c>
-      <c r="I15">
-        <v>0.03034157858539465</v>
-      </c>
-      <c r="J15">
-        <v>-0.006579688439123123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C16">
-        <v>0.003007863751965938</v>
+        <v>0.001620135616805425</v>
       </c>
       <c r="E16">
-        <v>-0.00968640992160248</v>
+        <v>0.007825959385038373</v>
       </c>
       <c r="F16">
-        <v>0.02518965929741482</v>
+        <v>-0.004067051682682067</v>
       </c>
       <c r="H16">
-        <v>-0.0252606288151572</v>
+        <v>0.004078764355150573</v>
       </c>
       <c r="I16">
-        <v>-0.01607945951986488</v>
+        <v>0.008303432108137283</v>
       </c>
       <c r="J16">
-        <v>-0.01546416018340198</v>
+        <v>-0.01956840203256883</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C17">
-        <v>0.003683102420775605</v>
+        <v>0.00136514549460582</v>
       </c>
       <c r="E17">
-        <v>0.001077483269370817</v>
+        <v>7.960320318412811E-06</v>
       </c>
       <c r="F17">
-        <v>-0.01070875017718754</v>
+        <v>-0.006272667994906719</v>
       </c>
       <c r="H17">
-        <v>0.01060242415060604</v>
+        <v>0.006518461796738471</v>
       </c>
       <c r="I17">
-        <v>0.001017133754283439</v>
+        <v>0.005896042603841703</v>
       </c>
       <c r="J17">
-        <v>0.01279853831731187</v>
+        <v>-0.004315955290631166</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C18">
-        <v>0.009939257484814371</v>
+        <v>0.01526795734671829</v>
       </c>
       <c r="E18">
-        <v>0.01604369051092263</v>
+        <v>0.002708669676346787</v>
       </c>
       <c r="F18">
-        <v>-0.01246069211517303</v>
+        <v>-0.001605290944211638</v>
       </c>
       <c r="H18">
-        <v>0.01244925611231403</v>
+        <v>0.00154255926170237</v>
       </c>
       <c r="I18">
-        <v>0.009544404886101221</v>
+        <v>-0.0002331010653240426</v>
       </c>
       <c r="J18">
-        <v>0.02187544633850829</v>
+        <v>0.007453877028566195</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C19">
-        <v>0.03152429138107284</v>
+        <v>0.005928089613123583</v>
       </c>
       <c r="E19">
-        <v>-0.01140801735200434</v>
+        <v>0.0006603959304158371</v>
       </c>
       <c r="F19">
-        <v>0.003143705285926321</v>
+        <v>0.000413647600545904</v>
       </c>
       <c r="H19">
-        <v>-0.003341723335430833</v>
+        <v>-0.0003596484623859385</v>
       </c>
       <c r="I19">
-        <v>-0.006618253654563414</v>
+        <v>0.002854861554194462</v>
       </c>
       <c r="J19">
-        <v>0.02099171666717349</v>
+        <v>-0.009818421305930008</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1034,22 +1039,22 @@
         <v>44</v>
       </c>
       <c r="C20">
-        <v>0.001218132304533076</v>
+        <v>-0.0181484401499376</v>
       </c>
       <c r="E20">
-        <v>-0.01941311135327784</v>
+        <v>-0.006156371478254857</v>
       </c>
       <c r="F20">
-        <v>0.02938678934669733</v>
+        <v>0.004868278370731134</v>
       </c>
       <c r="H20">
-        <v>-0.02944831936207985</v>
+        <v>-0.004806710400268415</v>
       </c>
       <c r="I20">
-        <v>-0.03183967695991924</v>
+        <v>-0.002026378833055153</v>
       </c>
       <c r="J20">
-        <v>0.003944168907142948</v>
+        <v>0.003543377342157545</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1058,304 +1063,328 @@
         <v>45</v>
       </c>
       <c r="C21">
-        <v>-0.01112019578004894</v>
+        <v>-0.022813675152547</v>
       </c>
       <c r="E21">
-        <v>-0.02678605419651355</v>
+        <v>0.0113808977032359</v>
       </c>
       <c r="F21">
-        <v>0.02868533217133305</v>
+        <v>-0.004949300357972013</v>
       </c>
       <c r="H21">
-        <v>-0.02887138471784618</v>
+        <v>0.005052600202104007</v>
       </c>
       <c r="I21">
-        <v>-0.03873141518285379</v>
+        <v>0.003556671886266875</v>
       </c>
       <c r="J21">
-        <v>0.02932160715811319</v>
+        <v>0.008196569064025674</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C22">
-        <v>-0.01374628693657174</v>
+        <v>-0.02214966990998679</v>
       </c>
       <c r="E22">
-        <v>4.129951032487758E-05</v>
+        <v>-0.01159324654372986</v>
       </c>
       <c r="F22">
-        <v>0.001811719952929988</v>
+        <v>0.01105747474629899</v>
       </c>
       <c r="H22">
-        <v>-0.001984150996037749</v>
+        <v>-0.01103848815353952</v>
       </c>
       <c r="I22">
-        <v>0.004501625625406406</v>
+        <v>-0.01086898229075929</v>
       </c>
       <c r="J22">
-        <v>-0.009121589531929685</v>
+        <v>0.006366690229209365</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C23">
-        <v>-0.02715441978860494</v>
+        <v>-0.004630091513203659</v>
       </c>
       <c r="E23">
-        <v>-0.02905618176404545</v>
+        <v>-0.01230116593204664</v>
       </c>
       <c r="F23">
-        <v>0.02108617577154394</v>
+        <v>0.01396085643043425</v>
       </c>
       <c r="H23">
-        <v>-0.02110525727631432</v>
+        <v>-0.01408289105931564</v>
       </c>
       <c r="I23">
-        <v>-0.02827631506907876</v>
+        <v>-0.01179273109570924</v>
       </c>
       <c r="J23">
-        <v>-0.02591206458928833</v>
+        <v>-0.01849373487128882</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C24">
-        <v>-0.004212524553131138</v>
+        <v>-0.009812086472483458</v>
       </c>
       <c r="E24">
-        <v>-0.02371696192924048</v>
+        <v>0.007106797916271916</v>
       </c>
       <c r="F24">
-        <v>0.03356786339196585</v>
+        <v>-0.01023005272920211</v>
       </c>
       <c r="H24">
-        <v>-0.03380995445248861</v>
+        <v>0.01027197593087904</v>
       </c>
       <c r="I24">
-        <v>-0.02136614634153658</v>
+        <v>0.01310582932423317</v>
       </c>
       <c r="J24">
-        <v>0.01968961512747397</v>
+        <v>0.004913271513563789</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C25">
-        <v>-0.02208698802174701</v>
+        <v>0.004657418106296723</v>
       </c>
       <c r="E25">
-        <v>-0.002294646573661643</v>
+        <v>0.01962831332913253</v>
       </c>
       <c r="F25">
-        <v>0.004760446190111547</v>
+        <v>-0.01705115981804639</v>
       </c>
       <c r="H25">
-        <v>-0.004793546698386674</v>
+        <v>0.01705464893818595</v>
       </c>
       <c r="I25">
-        <v>-0.01063446565861641</v>
+        <v>0.01985164889006595</v>
       </c>
       <c r="J25">
-        <v>0.03237794405419208</v>
+        <v>0.005847604250277086</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C26">
-        <v>-0.01951374337843585</v>
+        <v>0.02198199620727985</v>
       </c>
       <c r="E26">
-        <v>-0.006935349233837308</v>
+        <v>0.005956423246256929</v>
       </c>
       <c r="F26">
-        <v>0.003691886422971605</v>
+        <v>-0.01390672644426905</v>
       </c>
       <c r="H26">
-        <v>-0.00367884991971248</v>
+        <v>0.0138342625693705</v>
       </c>
       <c r="I26">
-        <v>0.001864071466017867</v>
+        <v>0.01161479844859194</v>
       </c>
       <c r="J26">
-        <v>-0.04633925368647526</v>
+        <v>-0.0129405840538354</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C27">
-        <v>-0.003142797785699446</v>
+        <v>0.02228941845957674</v>
       </c>
       <c r="E27">
-        <v>-0.02542533335633334</v>
+        <v>-0.02877250838290033</v>
       </c>
       <c r="F27">
-        <v>0.01774198193549548</v>
+        <v>0.02570396714015868</v>
       </c>
       <c r="H27">
-        <v>-0.01791548547887137</v>
+        <v>-0.02567916419516656</v>
       </c>
       <c r="I27">
-        <v>-0.02613039653259913</v>
+        <v>-0.0217181802287272</v>
       </c>
       <c r="J27">
-        <v>0.01620433948026695</v>
+        <v>0.001217981061547961</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C28">
-        <v>0.05938487684621921</v>
+        <v>-0.01376402301456092</v>
       </c>
       <c r="E28">
-        <v>-0.01949829937457484</v>
+        <v>0.01687623609904944</v>
       </c>
       <c r="F28">
-        <v>0.0104162156040539</v>
+        <v>-0.01179589208783568</v>
       </c>
       <c r="H28">
-        <v>-0.0104739476184869</v>
+        <v>0.0117324099732964</v>
       </c>
       <c r="I28">
-        <v>-0.0048133692033423</v>
+        <v>0.008258797386351895</v>
       </c>
       <c r="J28">
-        <v>-0.01669326753991083</v>
+        <v>-0.01671249160560131</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C29">
-        <v>-0.01184257796064449</v>
+        <v>0.01106015948240638</v>
       </c>
       <c r="E29">
-        <v>0.01455647763911941</v>
+        <v>-0.005511798460471938</v>
       </c>
       <c r="F29">
-        <v>0.001248730812182703</v>
+        <v>0.006316617468664697</v>
       </c>
       <c r="H29">
-        <v>-0.001344609336152334</v>
+        <v>-0.006353830718153227</v>
       </c>
       <c r="I29">
-        <v>0.003953183488295872</v>
+        <v>-0.008030665089226603</v>
       </c>
       <c r="J29">
-        <v>-0.01425650325372697</v>
+        <v>0.01089234380240115</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C30">
-        <v>-0.03624465756116439</v>
+        <v>0.003827297721091908</v>
       </c>
       <c r="E30">
-        <v>-0.01560615540153885</v>
+        <v>0.005009897960395917</v>
       </c>
       <c r="F30">
-        <v>0.02801751100437775</v>
+        <v>-0.002118199380727975</v>
       </c>
       <c r="H30">
-        <v>-0.02810288352572088</v>
+        <v>0.002111769396470776</v>
       </c>
       <c r="I30">
-        <v>-0.0253442508360627</v>
+        <v>0.003067178618687144</v>
       </c>
       <c r="J30">
-        <v>-0.002873680350950502</v>
+        <v>-0.021808116186103</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C31">
-        <v>-0.001529857882464471</v>
+        <v>-0.00755999828639993</v>
       </c>
       <c r="E31">
-        <v>0.004233539558384889</v>
+        <v>0.01726961963478478</v>
       </c>
       <c r="F31">
-        <v>-0.003400446850111712</v>
+        <v>-0.0209757651590306</v>
       </c>
       <c r="H31">
-        <v>0.003449708362427091</v>
+        <v>0.02101267216850689</v>
       </c>
       <c r="I31">
-        <v>0.008552372138093034</v>
+        <v>0.01505415967416639</v>
       </c>
       <c r="J31">
-        <v>0.003247015777780447</v>
+        <v>0.01263127517042416</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C32">
-        <v>-0.03115085128771283</v>
+        <v>0.008916752324670093</v>
       </c>
       <c r="E32">
-        <v>0.008799450699862675</v>
+        <v>0.003597134351885373</v>
       </c>
       <c r="F32">
-        <v>-0.009751983937995983</v>
+        <v>-0.00246115651444626</v>
       </c>
       <c r="H32">
-        <v>0.009643854910963727</v>
+        <v>0.002406348960253958</v>
       </c>
       <c r="I32">
-        <v>0.009905729476432368</v>
+        <v>0.00375449650217986</v>
       </c>
       <c r="J32">
-        <v>-0.008194478762290892</v>
+        <v>0.0007849565781093693</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33">
+        <v>0.006172791318911653</v>
+      </c>
+      <c r="E33">
+        <v>-0.001873426922937076</v>
+      </c>
+      <c r="F33">
+        <v>0.007547397325895891</v>
+      </c>
+      <c r="H33">
+        <v>-0.007615737328629492</v>
+      </c>
+      <c r="I33">
+        <v>-0.00460812575232503</v>
+      </c>
+      <c r="J33">
+        <v>0.002380971712721403</v>
       </c>
     </row>
   </sheetData>
@@ -1363,10 +1392,10 @@
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>